<commit_message>
Changes in handling addressbook
</commit_message>
<xml_diff>
--- a/fw_rules_test_02.xlsx
+++ b/fw_rules_test_02.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\fw-rule-manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BA6E73-3019-4976-B257-F3829DFB9503}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA45E8BD-64C0-4719-860B-1327C53F48CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="677" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34620" yWindow="3345" windowWidth="21615" windowHeight="10335" tabRatio="677" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Traffic Flows" sheetId="2" r:id="rId1"/>
-    <sheet name="Dropdown Fields" sheetId="4" r:id="rId2"/>
-    <sheet name="Instructions" sheetId="1" r:id="rId3"/>
+    <sheet name="Address Book" sheetId="5" r:id="rId2"/>
+    <sheet name="Dropdown Fields" sheetId="4" r:id="rId3"/>
+    <sheet name="Instructions" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Traffic Flows'!$A$1:$M$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Traffic Flows'!$A$1:$K$3</definedName>
     <definedName name="BulkData">'Dropdown Fields'!#REF!</definedName>
     <definedName name="Customer">'Dropdown Fields'!#REF!</definedName>
     <definedName name="DestinationProtocol">'Dropdown Fields'!#REF!</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="199">
   <si>
     <t>Source Network</t>
   </si>
@@ -89,12 +90,6 @@
     <t>YesNo</t>
   </si>
   <si>
-    <t>Destination Mask Length</t>
-  </si>
-  <si>
-    <t>Source Mask Length</t>
-  </si>
-  <si>
     <t>any</t>
   </si>
   <si>
@@ -134,30 +129,12 @@
     <t>Click and drag the bottom-right corner of the table to make it bigger</t>
   </si>
   <si>
-    <t>QoS Flows</t>
-  </si>
-  <si>
-    <t>To allow scripting of output into Cisco configuration, please create flow records that match the limits of what can be configured in an ACL entry</t>
-  </si>
-  <si>
-    <t>In client-server protocols like TCP this is significant. If you select Return then you are saying that server traffic will come back to the client through this trust boundary</t>
-  </si>
-  <si>
-    <t>Entry and Return are the directionality of a flow</t>
-  </si>
-  <si>
     <t>Protocol</t>
   </si>
   <si>
-    <t>Return flows need to swap source and destination addresses and also the destination port becomes the source port</t>
-  </si>
-  <si>
     <t>Genesys</t>
   </si>
   <si>
-    <t>AJW: Consider Shadowing and Optimisation</t>
-  </si>
-  <si>
     <t>Web Customer Facing Tools</t>
   </si>
   <si>
@@ -182,21 +159,9 @@
     <t>Comment:</t>
   </si>
   <si>
-    <t>Port ranges: Please separate numbers with a dash, i.e. 52000-52009</t>
-  </si>
-  <si>
-    <t>Teller and InterAct application Client to Server</t>
-  </si>
-  <si>
-    <t>Each service can only map to one QoS class, as otherwise scripting of configs may map all flows of service to one of the QoS classes specified so results may vary...</t>
-  </si>
-  <si>
     <t>EMC Centera Replication</t>
   </si>
   <si>
-    <t>In the "QoS Flows" Worksheet, select the first usable cell in the column then CTRL+SHIFT+Down Arrow to select to last possible value in column</t>
-  </si>
-  <si>
     <t>Voice Signalling</t>
   </si>
   <si>
@@ -209,35 +174,6 @@
     <t>Genesys Database Traffic</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Note: Layer-3 (IP) only flow specifications, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">that are done as pairs of rows for bi-directionality </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(ref mjh90-93 as example), should not have 'return' flags set as this causes duplicate ACEs from scripting</t>
-    </r>
-  </si>
-  <si>
-    <t>For layer-3 flows (i.e. no TCP or UDP definition), see note below as to why individual rows are required per direction, without a return specified</t>
-  </si>
-  <si>
     <t>Traffic to CFS servers</t>
   </si>
   <si>
@@ -301,24 +237,15 @@
     <t>Rule Name</t>
   </si>
   <si>
-    <t>TFTP</t>
-  </si>
-  <si>
     <t>10.64.0.0/16, 10.5.0.0/28</t>
   </si>
   <si>
-    <t>10.88.1.2/32, 172.1.0.0/16</t>
-  </si>
-  <si>
     <t>internal-management</t>
   </si>
   <si>
     <t>servers1</t>
   </si>
   <si>
-    <t>192.168.0.1/32, 172.27.28.0/29</t>
-  </si>
-  <si>
     <t>10.78.0.0/24</t>
   </si>
   <si>
@@ -329,6 +256,390 @@
   </si>
   <si>
     <t>internet-untrust</t>
+  </si>
+  <si>
+    <t>In the "Traffic Flows" Worksheet, select the first usable cell in the column then CTRL+SHIFT+Down Arrow to select to last possible value in column</t>
+  </si>
+  <si>
+    <t>Management SSH</t>
+  </si>
+  <si>
+    <t>SSH from Management Network</t>
+  </si>
+  <si>
+    <t>globtftp01</t>
+  </si>
+  <si>
+    <t>172.16.40.24/32</t>
+  </si>
+  <si>
+    <t>esbu-172-supernet</t>
+  </si>
+  <si>
+    <t>172.16.0.0/12</t>
+  </si>
+  <si>
+    <t>azure-aus-jumphost</t>
+  </si>
+  <si>
+    <t>10.248.58.128/26</t>
+  </si>
+  <si>
+    <t>azure-aue-jumphost</t>
+  </si>
+  <si>
+    <t>10.248.56.128/26</t>
+  </si>
+  <si>
+    <t>azure-aus-aue-supernet</t>
+  </si>
+  <si>
+    <t>10.248.56.0/21</t>
+  </si>
+  <si>
+    <t>portpuppet01</t>
+  </si>
+  <si>
+    <t>172.21.40.129/32</t>
+  </si>
+  <si>
+    <t>globswsat01</t>
+  </si>
+  <si>
+    <t>172.16.40.72/32</t>
+  </si>
+  <si>
+    <t>portswsat01</t>
+  </si>
+  <si>
+    <t>172.21.40.72/32</t>
+  </si>
+  <si>
+    <t>azure-aus-spacewalk</t>
+  </si>
+  <si>
+    <t>10.248.59.20/32</t>
+  </si>
+  <si>
+    <t>azure-aue-spacewalk</t>
+  </si>
+  <si>
+    <t>10.248.57.20/32</t>
+  </si>
+  <si>
+    <t>azure-aue-ad-group</t>
+  </si>
+  <si>
+    <t>10.248.56.192/26</t>
+  </si>
+  <si>
+    <t>azure-aus-ad-group</t>
+  </si>
+  <si>
+    <t>10.248.58.192/26</t>
+  </si>
+  <si>
+    <t>globrhsat01</t>
+  </si>
+  <si>
+    <t>172.16.40.226/32</t>
+  </si>
+  <si>
+    <t>portrhsat01</t>
+  </si>
+  <si>
+    <t>172.21.40.226/32</t>
+  </si>
+  <si>
+    <t>globdcs01</t>
+  </si>
+  <si>
+    <t>172.17.6.20/32</t>
+  </si>
+  <si>
+    <t>globdcs02</t>
+  </si>
+  <si>
+    <t>172.17.6.21/32</t>
+  </si>
+  <si>
+    <t>azure-aus-redhat01</t>
+  </si>
+  <si>
+    <t>10.248.59.21/32</t>
+  </si>
+  <si>
+    <t>azure-aue-redhat01</t>
+  </si>
+  <si>
+    <t>10.248.57.21/32</t>
+  </si>
+  <si>
+    <t>portdcs02</t>
+  </si>
+  <si>
+    <t>172.21.6.21/32</t>
+  </si>
+  <si>
+    <t>portdcs01</t>
+  </si>
+  <si>
+    <t>172.21.6.20/32</t>
+  </si>
+  <si>
+    <t>portrepo01</t>
+  </si>
+  <si>
+    <t>172.21.40.21/32</t>
+  </si>
+  <si>
+    <t>globansible01</t>
+  </si>
+  <si>
+    <t>172.16.40.133/32</t>
+  </si>
+  <si>
+    <t>azure-host-10.248.56.200</t>
+  </si>
+  <si>
+    <t>10.248.56.200/32</t>
+  </si>
+  <si>
+    <t>azure-host-10.248.56.201</t>
+  </si>
+  <si>
+    <t>10.248.56.201/32</t>
+  </si>
+  <si>
+    <t>globca01</t>
+  </si>
+  <si>
+    <t>172.17.6.40/32</t>
+  </si>
+  <si>
+    <t>aueats01</t>
+  </si>
+  <si>
+    <t>10.248.56.150/32</t>
+  </si>
+  <si>
+    <t>aueats02</t>
+  </si>
+  <si>
+    <t>10.248.56.151/32</t>
+  </si>
+  <si>
+    <t>ausets01</t>
+  </si>
+  <si>
+    <t>10.248.58.150/32</t>
+  </si>
+  <si>
+    <t>ausets02</t>
+  </si>
+  <si>
+    <t>10.248.58.151/32</t>
+  </si>
+  <si>
+    <t>globkms01</t>
+  </si>
+  <si>
+    <t>172.16.40.10/32</t>
+  </si>
+  <si>
+    <t>aueagraylog01</t>
+  </si>
+  <si>
+    <t>10.248.57.30/32</t>
+  </si>
+  <si>
+    <t>aueagraylog02</t>
+  </si>
+  <si>
+    <t>10.248.57.31/32</t>
+  </si>
+  <si>
+    <t>aueagraylog03</t>
+  </si>
+  <si>
+    <t>10.248.57.32/32</t>
+  </si>
+  <si>
+    <t>aueagraylog04</t>
+  </si>
+  <si>
+    <t>10.248.57.33/32</t>
+  </si>
+  <si>
+    <t>globkafka01</t>
+  </si>
+  <si>
+    <t>172.17.7.239/32</t>
+  </si>
+  <si>
+    <t>globkafka02</t>
+  </si>
+  <si>
+    <t>172.17.7.244/32</t>
+  </si>
+  <si>
+    <t>globkafka03</t>
+  </si>
+  <si>
+    <t>172.17.7.247/32</t>
+  </si>
+  <si>
+    <t>globkafka04</t>
+  </si>
+  <si>
+    <t>172.17.7.123/32</t>
+  </si>
+  <si>
+    <t>globkafka05</t>
+  </si>
+  <si>
+    <t>172.17.7.126/32</t>
+  </si>
+  <si>
+    <t>globkafka06</t>
+  </si>
+  <si>
+    <t>172.17.7.131/32</t>
+  </si>
+  <si>
+    <t>globgraylog11</t>
+  </si>
+  <si>
+    <t>172.17.7.9/32</t>
+  </si>
+  <si>
+    <t>globgraylog12</t>
+  </si>
+  <si>
+    <t>172.17.7.17/32</t>
+  </si>
+  <si>
+    <t>globgraylog13</t>
+  </si>
+  <si>
+    <t>172.17.7.22/32</t>
+  </si>
+  <si>
+    <t>globgraylog14</t>
+  </si>
+  <si>
+    <t>172.17.7.30/32</t>
+  </si>
+  <si>
+    <t>globgraylog15</t>
+  </si>
+  <si>
+    <t>172.17.7.32/32</t>
+  </si>
+  <si>
+    <t>globgraylog16</t>
+  </si>
+  <si>
+    <t>172.17.7.39/32</t>
+  </si>
+  <si>
+    <t>globgraylog17</t>
+  </si>
+  <si>
+    <t>172.17.7.44/32</t>
+  </si>
+  <si>
+    <t>globgraylog18</t>
+  </si>
+  <si>
+    <t>172.17.7.47/32</t>
+  </si>
+  <si>
+    <t>aueafrmnprxy01</t>
+  </si>
+  <si>
+    <t>10.248.57.50/32</t>
+  </si>
+  <si>
+    <t>globforeman01</t>
+  </si>
+  <si>
+    <t>172.17.7.138/32</t>
+  </si>
+  <si>
+    <t>globforeman02</t>
+  </si>
+  <si>
+    <t>172.17.7.129/32</t>
+  </si>
+  <si>
+    <t>aueapuppet01</t>
+  </si>
+  <si>
+    <t>ausepuppet01</t>
+  </si>
+  <si>
+    <t>10.248.59.50/32</t>
+  </si>
+  <si>
+    <t>globgit01</t>
+  </si>
+  <si>
+    <t>172.16.40.19/32</t>
+  </si>
+  <si>
+    <t>cbus-aapt-wan</t>
+  </si>
+  <si>
+    <t>172.22.0.0/24</t>
+  </si>
+  <si>
+    <t>cbus-aapt-tloc-172.23.0.0/24</t>
+  </si>
+  <si>
+    <t>172.23.0.0/24</t>
+  </si>
+  <si>
+    <t>globdwannetutil02</t>
+  </si>
+  <si>
+    <t>118.127.84.2/32</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>ESBU TFTP</t>
+  </si>
+  <si>
+    <t>Azure Mgmt Hosts Net 1</t>
+  </si>
+  <si>
+    <t>Azure Mgmt Hosts Net 2</t>
+  </si>
+  <si>
+    <t>globansible01, portpuppet01</t>
+  </si>
+  <si>
+    <t>InterAct application Client to Server</t>
+  </si>
+  <si>
+    <t>SSH access from Management Infra Services</t>
+  </si>
+  <si>
+    <t>Management SSH Infra Services</t>
+  </si>
+  <si>
+    <t>Object Name</t>
+  </si>
+  <si>
+    <t>172.27.28.0/29, globdcs01</t>
+  </si>
+  <si>
+    <t>88.3.98.2/32, aueapuppet01</t>
+  </si>
+  <si>
+    <t>azure-aus-redhat01, 10.1.2.0/24</t>
   </si>
 </sst>
 </file>
@@ -373,7 +684,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -398,8 +709,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -422,11 +739,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -460,29 +792,12 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -551,31 +866,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -587,137 +878,13 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF669900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF89B0FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
-        <color theme="0"/>
+        <b/>
+        <i val="0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF006600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3379CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF669900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF89B0FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF006600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3379CD"/>
         </patternFill>
       </fill>
     </dxf>
@@ -777,7 +944,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>201930</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
@@ -1198,295 +1365,266 @@
     <tabColor rgb="FF33CC33"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="46.109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" style="11" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="28.77734375" style="8" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" style="8" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="21.77734375" style="11" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" style="8" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" style="8" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="10" style="8" customWidth="1"/>
-    <col min="11" max="11" width="14" style="11" customWidth="1"/>
-    <col min="12" max="12" width="9" style="8" customWidth="1"/>
-    <col min="13" max="13" width="10.33203125" style="5" customWidth="1"/>
-    <col min="14" max="16384" width="9.109375" style="8"/>
+    <col min="1" max="1" width="30" style="8" customWidth="1"/>
+    <col min="2" max="2" width="41.77734375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" style="11" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="39.33203125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="10" style="8" customWidth="1"/>
+    <col min="9" max="9" width="14" style="11" customWidth="1"/>
+    <col min="10" max="10" width="9" style="8" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" style="5" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>59</v>
+      <c r="F1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="D2" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="10">
+        <v>50410</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="B3" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="6">
-        <v>0</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="I2" s="6">
-        <v>16</v>
-      </c>
-      <c r="J2" s="6" t="s">
+      <c r="H3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="10">
+        <v>5389</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="10">
-        <v>50410</v>
-      </c>
-      <c r="L2" s="6" t="s">
+      <c r="I4" s="10">
+        <v>443</v>
+      </c>
+      <c r="J4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="K4" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="10">
+        <v>22</v>
+      </c>
+      <c r="J5" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="K5" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="6">
-        <v>0</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="I3" s="6">
-        <v>16</v>
-      </c>
-      <c r="J3" s="6" t="s">
+      <c r="G6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="10">
-        <v>5388</v>
-      </c>
-      <c r="L3" s="6" t="s">
+      <c r="I6" s="10">
+        <v>22</v>
+      </c>
+      <c r="J6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="I4" s="6">
-        <v>16</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="10">
-        <v>443</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="6">
-        <v>16</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="10">
-        <v>69</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>6</v>
+      <c r="K6" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="L2:L3 L6:L1048576">
-    <cfRule type="cellIs" dxfId="33" priority="4274" operator="equal">
+  <autoFilter ref="A1:K3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="J2:J1048576">
+    <cfRule type="cellIs" dxfId="11" priority="4278" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="4275" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="4279" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M3">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+  <conditionalFormatting sqref="K2:K6">
+    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L4">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M4">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L5">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M5">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="14" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M5 L2:L1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K6 J2:J1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>INDIRECT("Boolean[Column1]")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C6 C7:D1048576 H2:H1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>INDIRECT("DestProtoTable[Column1]")</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>INDIRECT("ServiceTable[Column1]")</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C5 C6:D1048576 J2:J1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>INDIRECT("DestProtoTable[Column1]")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -1498,7 +1636,7 @@
           <x14:formula1>
             <xm:f>'Dropdown Fields'!$N$2:$N$9</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D5 G2:G5</xm:sqref>
+          <xm:sqref>D2:D6 F2:F6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1507,6 +1645,506 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4DD4B2-3C11-488A-8A79-AB6EEFDFC7EF}">
+  <sheetPr>
+    <tabColor rgb="FF7030A0"/>
+  </sheetPr>
+  <dimension ref="A1:C58"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>126</v>
+      </c>
+      <c r="B28" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>128</v>
+      </c>
+      <c r="B29" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>130</v>
+      </c>
+      <c r="B30" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>132</v>
+      </c>
+      <c r="B31" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>134</v>
+      </c>
+      <c r="B32" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B33" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>138</v>
+      </c>
+      <c r="B34" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>140</v>
+      </c>
+      <c r="B35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>142</v>
+      </c>
+      <c r="B36" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>144</v>
+      </c>
+      <c r="B37" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>146</v>
+      </c>
+      <c r="B38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>148</v>
+      </c>
+      <c r="B39" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>150</v>
+      </c>
+      <c r="B40" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>152</v>
+      </c>
+      <c r="B41" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>154</v>
+      </c>
+      <c r="B42" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>156</v>
+      </c>
+      <c r="B43" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>158</v>
+      </c>
+      <c r="B44" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>160</v>
+      </c>
+      <c r="B45" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>162</v>
+      </c>
+      <c r="B46" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>164</v>
+      </c>
+      <c r="B47" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>166</v>
+      </c>
+      <c r="B48" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>168</v>
+      </c>
+      <c r="B49" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>170</v>
+      </c>
+      <c r="B50" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>172</v>
+      </c>
+      <c r="B51" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>174</v>
+      </c>
+      <c r="B52" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>176</v>
+      </c>
+      <c r="B53" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>177</v>
+      </c>
+      <c r="B54" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>179</v>
+      </c>
+      <c r="B55" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>181</v>
+      </c>
+      <c r="B56" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>183</v>
+      </c>
+      <c r="B57" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>185</v>
+      </c>
+      <c r="B58" t="s">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FFCCECFF"/>
@@ -1514,7 +2152,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1535,13 +2173,13 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>14</v>
@@ -1550,24 +2188,24 @@
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M1" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="N1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -1579,15 +2217,15 @@
         <v>6</v>
       </c>
       <c r="N2" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -1596,120 +2234,120 @@
         <v>9</v>
       </c>
       <c r="N3" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
       </c>
       <c r="N4" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
       </c>
       <c r="N5" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="O5" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="N6" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="O6" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="N7" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="O7" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="N8" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="O8" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="N9" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="O9" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1725,27 +2363,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet5">
     <tabColor theme="2" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1753,7 +2391,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1761,7 +2399,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1769,7 +2407,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1777,12 +2415,12 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -1790,7 +2428,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -1798,7 +2436,7 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1806,7 +2444,7 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -1814,17 +2452,17 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -1841,56 +2479,6 @@
       </c>
       <c r="B29" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A32" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C35" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C36" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C37" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added multiple zones, fixed bug when policy is enabled and menawhile deleted
</commit_message>
<xml_diff>
--- a/fw_rules_test_02.xlsx
+++ b/fw_rules_test_02.xlsx
@@ -8,27 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\fw-rule-manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA45E8BD-64C0-4719-860B-1327C53F48CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7824DF-8B64-4785-82AC-62D72E0FD1B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34620" yWindow="3345" windowWidth="21615" windowHeight="10335" tabRatio="677" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="647" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Traffic Flows" sheetId="2" r:id="rId1"/>
     <sheet name="Address Book" sheetId="5" r:id="rId2"/>
-    <sheet name="Dropdown Fields" sheetId="4" r:id="rId3"/>
-    <sheet name="Instructions" sheetId="1" r:id="rId4"/>
+    <sheet name="Standard Apps" sheetId="7" r:id="rId3"/>
+    <sheet name="Zones" sheetId="8" r:id="rId4"/>
+    <sheet name="Dropdown Fields" sheetId="4" r:id="rId5"/>
+    <sheet name="Instructions" sheetId="1" r:id="rId6"/>
+    <sheet name="Feedback" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Traffic Flows'!$A$1:$K$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Traffic Flows'!$A$1:$K$8</definedName>
     <definedName name="BulkData">'Dropdown Fields'!#REF!</definedName>
     <definedName name="Customer">'Dropdown Fields'!#REF!</definedName>
     <definedName name="DestinationProtocol">'Dropdown Fields'!#REF!</definedName>
-    <definedName name="DestProto">'Dropdown Fields'!$E:$E</definedName>
+    <definedName name="DestProto">'Dropdown Fields'!$B:$B</definedName>
     <definedName name="QoSClass">'Dropdown Fields'!#REF!</definedName>
-    <definedName name="Service">'Dropdown Fields'!$B:$B</definedName>
+    <definedName name="Service">'Dropdown Fields'!#REF!</definedName>
     <definedName name="SourceDSCP">'Dropdown Fields'!#REF!</definedName>
     <definedName name="TimeSensitive">'Dropdown Fields'!#REF!</definedName>
-    <definedName name="YesNo">'Dropdown Fields'!$H:$H</definedName>
+    <definedName name="YesNo">'Dropdown Fields'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="273">
   <si>
     <t>Source Network</t>
   </si>
@@ -57,9 +60,6 @@
     <t>Destination Port</t>
   </si>
   <si>
-    <t>Service</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -87,9 +87,6 @@
     <t>IPSec</t>
   </si>
   <si>
-    <t>YesNo</t>
-  </si>
-  <si>
     <t>any</t>
   </si>
   <si>
@@ -132,48 +129,18 @@
     <t>Protocol</t>
   </si>
   <si>
-    <t>Genesys</t>
-  </si>
-  <si>
-    <t>Web Customer Facing Tools</t>
-  </si>
-  <si>
-    <t>Intranet Sites</t>
-  </si>
-  <si>
     <t>Internet Browsing</t>
   </si>
   <si>
     <t>Digital Media Content</t>
   </si>
   <si>
-    <t>Domain Logon</t>
-  </si>
-  <si>
-    <t>eCRS</t>
-  </si>
-  <si>
-    <t>ePO</t>
-  </si>
-  <si>
     <t>Comment:</t>
   </si>
   <si>
-    <t>EMC Centera Replication</t>
-  </si>
-  <si>
-    <t>Voice Signalling</t>
-  </si>
-  <si>
-    <t>Voice TFTP</t>
-  </si>
-  <si>
     <t>Voice Genesys LCA</t>
   </si>
   <si>
-    <t>Genesys Database Traffic</t>
-  </si>
-  <si>
     <t>Traffic to CFS servers</t>
   </si>
   <si>
@@ -183,9 +150,6 @@
     <t>Destination Zone</t>
   </si>
   <si>
-    <t>Zone</t>
-  </si>
-  <si>
     <t>dmz1</t>
   </si>
   <si>
@@ -249,12 +213,6 @@
     <t>10.78.0.0/24</t>
   </si>
   <si>
-    <t>RDP Servers</t>
-  </si>
-  <si>
-    <t>DHCP Servers</t>
-  </si>
-  <si>
     <t>internet-untrust</t>
   </si>
   <si>
@@ -267,12 +225,12 @@
     <t>SSH from Management Network</t>
   </si>
   <si>
+    <t>88.3.98.2/32</t>
+  </si>
+  <si>
     <t>globtftp01</t>
   </si>
   <si>
-    <t>172.16.40.24/32</t>
-  </si>
-  <si>
     <t>esbu-172-supernet</t>
   </si>
   <si>
@@ -300,9 +258,6 @@
     <t>portpuppet01</t>
   </si>
   <si>
-    <t>172.21.40.129/32</t>
-  </si>
-  <si>
     <t>globswsat01</t>
   </si>
   <si>
@@ -318,15 +273,9 @@
     <t>azure-aus-spacewalk</t>
   </si>
   <si>
-    <t>10.248.59.20/32</t>
-  </si>
-  <si>
     <t>azure-aue-spacewalk</t>
   </si>
   <si>
-    <t>10.248.57.20/32</t>
-  </si>
-  <si>
     <t>azure-aue-ad-group</t>
   </si>
   <si>
@@ -396,9 +345,6 @@
     <t>globansible01</t>
   </si>
   <si>
-    <t>172.16.40.133/32</t>
-  </si>
-  <si>
     <t>azure-host-10.248.56.200</t>
   </si>
   <si>
@@ -633,13 +579,292 @@
     <t>Object Name</t>
   </si>
   <si>
-    <t>172.27.28.0/29, globdcs01</t>
-  </si>
-  <si>
     <t>88.3.98.2/32, aueapuppet01</t>
   </si>
   <si>
-    <t>azure-aus-redhat01, 10.1.2.0/24</t>
+    <t>test-segment</t>
+  </si>
+  <si>
+    <t>Test servers</t>
+  </si>
+  <si>
+    <t>172.27.28.0/29</t>
+  </si>
+  <si>
+    <t>azure-aus-redhat01, 10.1.2.0/24, aueafrmnprxy01</t>
+  </si>
+  <si>
+    <t>Management FTP Infra Services</t>
+  </si>
+  <si>
+    <t>FTP from Management Infra Services</t>
+  </si>
+  <si>
+    <t>address book - FQDNs</t>
+  </si>
+  <si>
+    <t>standard JUNOS app names</t>
+  </si>
+  <si>
+    <t>automatic application to FWs - Jenkins/Ansible</t>
+  </si>
+  <si>
+    <t>review process</t>
+  </si>
+  <si>
+    <t>explicit deny or action - log, etc</t>
+  </si>
+  <si>
+    <t>any zone - create global rule</t>
+  </si>
+  <si>
+    <t>dashes instead of _</t>
+  </si>
+  <si>
+    <t>if mask is /32 use host-</t>
+  </si>
+  <si>
+    <t>rules order - check</t>
+  </si>
+  <si>
+    <t>port ranges and list</t>
+  </si>
+  <si>
+    <t>tcp</t>
+  </si>
+  <si>
+    <t>junos-netbios-session</t>
+  </si>
+  <si>
+    <t>junos-smb-session</t>
+  </si>
+  <si>
+    <t>junos-ssh</t>
+  </si>
+  <si>
+    <t>junos-telnet</t>
+  </si>
+  <si>
+    <t>junos-smtp</t>
+  </si>
+  <si>
+    <t>junos-tacacs</t>
+  </si>
+  <si>
+    <t>junos-tacacs-ds</t>
+  </si>
+  <si>
+    <t>udp</t>
+  </si>
+  <si>
+    <t>junos-dhcp-client</t>
+  </si>
+  <si>
+    <t>junos-dhcp-server</t>
+  </si>
+  <si>
+    <t>junos-bootpc</t>
+  </si>
+  <si>
+    <t>junos-bootps</t>
+  </si>
+  <si>
+    <t>junos-finger</t>
+  </si>
+  <si>
+    <t>junos-http</t>
+  </si>
+  <si>
+    <t>junos-https</t>
+  </si>
+  <si>
+    <t>junos-pop3</t>
+  </si>
+  <si>
+    <t>junos-ident</t>
+  </si>
+  <si>
+    <t>junos-nntp</t>
+  </si>
+  <si>
+    <t>junos-ntp</t>
+  </si>
+  <si>
+    <t>junos-imap</t>
+  </si>
+  <si>
+    <t>junos-imaps</t>
+  </si>
+  <si>
+    <t>junos-bgp</t>
+  </si>
+  <si>
+    <t>junos-ldap</t>
+  </si>
+  <si>
+    <t>junos-snpp</t>
+  </si>
+  <si>
+    <t>junos-biff</t>
+  </si>
+  <si>
+    <t>junos-who</t>
+  </si>
+  <si>
+    <t>junos-syslog</t>
+  </si>
+  <si>
+    <t>junos-printer</t>
+  </si>
+  <si>
+    <t>junos-rip</t>
+  </si>
+  <si>
+    <t>junos-radius</t>
+  </si>
+  <si>
+    <t>junos-radacct</t>
+  </si>
+  <si>
+    <t>junos-nfsd-tcp</t>
+  </si>
+  <si>
+    <t>junos-nfsd-udp</t>
+  </si>
+  <si>
+    <t>junos-cvspserver</t>
+  </si>
+  <si>
+    <t>junos-ldp-tcp</t>
+  </si>
+  <si>
+    <t>junos-ldp-udp</t>
+  </si>
+  <si>
+    <t>junos-ike</t>
+  </si>
+  <si>
+    <t>junos-chargen</t>
+  </si>
+  <si>
+    <t>junos-dhcp-relay</t>
+  </si>
+  <si>
+    <t>junos-discard</t>
+  </si>
+  <si>
+    <t>junos-dns-udp</t>
+  </si>
+  <si>
+    <t>junos-dns-tcp</t>
+  </si>
+  <si>
+    <t>junos-echo</t>
+  </si>
+  <si>
+    <t>junos-gopher</t>
+  </si>
+  <si>
+    <t>junos-internet-locator-service</t>
+  </si>
+  <si>
+    <t>junos-ike-nat</t>
+  </si>
+  <si>
+    <t>junos-l2tp</t>
+  </si>
+  <si>
+    <t>junos-lpr</t>
+  </si>
+  <si>
+    <t>junos-mail</t>
+  </si>
+  <si>
+    <t>junos-msn</t>
+  </si>
+  <si>
+    <t>junos-ms-sql</t>
+  </si>
+  <si>
+    <t>junos-nbname</t>
+  </si>
+  <si>
+    <t>junos-nbds</t>
+  </si>
+  <si>
+    <t>junos-nfs</t>
+  </si>
+  <si>
+    <t>junos-nsm</t>
+  </si>
+  <si>
+    <t>junos-pc-anywhere</t>
+  </si>
+  <si>
+    <t>junos-sql-monitor</t>
+  </si>
+  <si>
+    <t>junos-sqlnet-v1</t>
+  </si>
+  <si>
+    <t>junos-sqlnet-v2</t>
+  </si>
+  <si>
+    <t>junos-smtps</t>
+  </si>
+  <si>
+    <t>junos-rdp</t>
+  </si>
+  <si>
+    <t>JUNOS-Name</t>
+  </si>
+  <si>
+    <t>Port</t>
+  </si>
+  <si>
+    <t>globansible01.esbu.local</t>
+  </si>
+  <si>
+    <t>globtftp01.esbu.local</t>
+  </si>
+  <si>
+    <t>portpuppet01.esbu.local</t>
+  </si>
+  <si>
+    <t>azure-serv-aus1.azure.net</t>
+  </si>
+  <si>
+    <t>azure-serv-aue1.azure.net</t>
+  </si>
+  <si>
+    <t>don't generate active if delete or active is there</t>
+  </si>
+  <si>
+    <t>Zone Name</t>
+  </si>
+  <si>
+    <t>Zone Set</t>
+  </si>
+  <si>
+    <t>internal1, internal2</t>
+  </si>
+  <si>
+    <t>dmz1, dmz2, internal1, internal2, servers1, internet-untrust</t>
+  </si>
+  <si>
+    <t>customer all zones</t>
+  </si>
+  <si>
+    <t>customer all internal zones</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>all-customer</t>
+  </si>
+  <si>
+    <t>all-internal</t>
   </si>
 </sst>
 </file>
@@ -684,7 +909,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -715,8 +940,14 @@
         <bgColor theme="4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF33CC33"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -754,11 +985,73 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -793,11 +1086,49 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -866,24 +1197,6 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -910,16 +1223,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF33CC33"/>
+      <color rgb="FFFF7171"/>
+      <color rgb="FFFFCC00"/>
       <color rgb="FFCCECFF"/>
-      <color rgb="FF33CC33"/>
       <color rgb="FF3379CD"/>
       <color rgb="FF006600"/>
       <color rgb="FF89B0FF"/>
       <color rgb="FF669900"/>
-      <color rgb="FFFFCC00"/>
       <color rgb="FFCC9900"/>
       <color rgb="FF6699FF"/>
-      <color rgb="FF008080"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1000,8 +1313,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Boolean" displayName="Boolean" ref="K1:K3" totalsRowShown="0">
-  <autoFilter ref="K1:K3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0CBA89D6-2693-40D7-8303-F1C744979C03}" name="Boolean104" displayName="Boolean104" ref="A1:C13" totalsRowShown="0">
+  <autoFilter ref="A1:C13" xr:uid="{AB4B5134-6824-485F-9F47-8D8A7CA67932}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{6988F3E5-D080-491E-8272-78CEDDC891B9}" name="Zone Name"/>
+    <tableColumn id="3" xr3:uid="{6BAFF4A9-DA69-4132-96EE-4BCBAB6EC3C6}" name="Zone Set"/>
+    <tableColumn id="2" xr3:uid="{55518FE0-84A0-40A9-AAFF-A81147B7E0D2}" name="Comment:"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Boolean" displayName="Boolean" ref="E1:E3" totalsRowShown="0">
+  <autoFilter ref="E1:E3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
   </tableColumns>
@@ -1009,32 +1334,11 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="DestProtoTable" displayName="DestProtoTable" ref="E1:E6" totalsRowShown="0">
-  <autoFilter ref="E1:E6" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="DestProtoTable" displayName="DestProtoTable" ref="B1:B6" totalsRowShown="0">
+  <autoFilter ref="B1:B6" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Column1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="ServiceTable" displayName="ServiceTable" ref="B1:B16" totalsRowShown="0">
-  <autoFilter ref="B1:B16" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Column1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{AEBF8D8A-9881-470F-9654-9DE70836114C}" name="Boolean10" displayName="Boolean10" ref="N1:O9" totalsRowShown="0">
-  <autoFilter ref="N1:O9" xr:uid="{33978E0E-0D46-4097-B840-A97054182E79}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{1D67A06E-EBD1-49A3-A9EE-3CBD65B4A34A}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{8E702BF8-30DE-4834-8652-5DEC7AED37AA}" name="Comment:"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1365,11 +1669,11 @@
     <tabColor rgb="FF33CC33"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1377,9 +1681,9 @@
     <col min="1" max="1" width="30" style="8" customWidth="1"/>
     <col min="2" max="2" width="41.77734375" style="5" customWidth="1"/>
     <col min="3" max="3" width="10.21875" style="11" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="39.33203125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="44.6640625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" style="11" customWidth="1"/>
     <col min="7" max="7" width="28.6640625" style="8" customWidth="1"/>
     <col min="8" max="8" width="10" style="8" customWidth="1"/>
     <col min="9" max="9" width="14" style="11" customWidth="1"/>
@@ -1390,130 +1694,130 @@
   <sheetData>
     <row r="1" spans="1:11" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>70</v>
+        <v>271</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I2" s="10">
         <v>50410</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I3" s="10">
         <v>5389</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>50</v>
+        <v>272</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>70</v>
+        <v>271</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>197</v>
+        <v>59</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>10</v>
@@ -1522,108 +1826,188 @@
         <v>443</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>65</v>
+        <v>272</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>15</v>
+        <v>180</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>15</v>
+        <v>177</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I5" s="10">
-        <v>22</v>
+        <v>443</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>191</v>
+        <v>98</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I6" s="10">
+        <v>21</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="10">
         <v>22</v>
       </c>
-      <c r="J6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="K6" s="6" t="s">
+      <c r="J7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>9</v>
       </c>
+      <c r="I8" s="10">
+        <v>22</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:K8" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="J2:J1048576">
-    <cfRule type="cellIs" dxfId="11" priority="4278" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4288" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4279" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4289" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K6">
-    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
+  <conditionalFormatting sqref="K2:K8">
+    <cfRule type="cellIs" dxfId="11" priority="23" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="24" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D8">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"any"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F8">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"any"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K6 J2:J1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576 K2:K8" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>INDIRECT("Boolean[Column1]")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C6 C7:D1048576 H2:H1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:D1048576 C2:C8 H2:H1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>INDIRECT("DestProtoTable[Column1]")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9:A1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>INDIRECT("ServiceTable[Column1]")</formula1>
     </dataValidation>
   </dataValidations>
@@ -1631,12 +2015,18 @@
   <pageSetup paperSize="8" scale="46" fitToHeight="8" orientation="landscape" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B6439085-EB4B-4087-9F04-35CF8BF8807D}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2B6C0FFB-6446-48FD-8F07-81E2C1CC72E5}">
           <x14:formula1>
-            <xm:f>'Dropdown Fields'!$N$2:$N$9</xm:f>
+            <xm:f>Zones!$A$2:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D6 F2:F6</xm:sqref>
+          <xm:sqref>F2:F8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8F8FD5C4-684E-44BA-98C0-2FC038D08AE1}">
+          <x14:formula1>
+            <xm:f>Zones!$A$2:$A$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D8</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1651,491 +2041,491 @@
   </sheetPr>
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.21875" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
     <col min="3" max="3" width="23.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>259</v>
       </c>
       <c r="C2" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>91</v>
+        <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>93</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="B14" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="B16" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="B17" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="B18" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="B19" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="B20" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="B21" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="B22" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="B23" t="s">
-        <v>117</v>
+        <v>258</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="B24" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="B25" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="B26" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="B27" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="B28" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="B29" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="B30" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="B31" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="B32" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="B33" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="B34" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="B35" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="B36" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="B37" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="B38" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="B39" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="B40" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="B41" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="B42" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="B43" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="B44" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="B45" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="B46" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="B47" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="B48" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="B49" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="B50" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="B51" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="B52" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="B53" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="B54" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="B55" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="B56" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="B57" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="B58" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2145,225 +2535,952 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7C7E070-0DF1-46AD-B71D-FFAED45E81B9}">
+  <sheetPr>
+    <tabColor rgb="FFFFCC00"/>
+  </sheetPr>
+  <dimension ref="A1:C62"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.44140625" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" s="20">
+        <v>139</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" s="20">
+        <v>445</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B4" s="20">
+        <v>22</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B5" s="20">
+        <v>23</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>194</v>
+      </c>
+      <c r="B6" s="20">
+        <v>25</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B7" s="20">
+        <v>49</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B8" s="20">
+        <v>65</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B9" s="20">
+        <v>68</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>202</v>
+      </c>
+      <c r="B10" s="20">
+        <v>67</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>202</v>
+      </c>
+      <c r="B11" s="20">
+        <v>68</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>202</v>
+      </c>
+      <c r="B12" s="20">
+        <v>67</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>194</v>
+      </c>
+      <c r="B13" s="20">
+        <v>79</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>194</v>
+      </c>
+      <c r="B14" s="20">
+        <v>80</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>194</v>
+      </c>
+      <c r="B15" s="20">
+        <v>443</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>194</v>
+      </c>
+      <c r="B16" s="20">
+        <v>110</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>194</v>
+      </c>
+      <c r="B17" s="20">
+        <v>113</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>194</v>
+      </c>
+      <c r="B18" s="20">
+        <v>119</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>202</v>
+      </c>
+      <c r="B19" s="20">
+        <v>123</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>194</v>
+      </c>
+      <c r="B20" s="20">
+        <v>143</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>194</v>
+      </c>
+      <c r="B21" s="20">
+        <v>993</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>194</v>
+      </c>
+      <c r="B22" s="20">
+        <v>179</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>194</v>
+      </c>
+      <c r="B23" s="20">
+        <v>389</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>194</v>
+      </c>
+      <c r="B24" s="20">
+        <v>444</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>202</v>
+      </c>
+      <c r="B25" s="20">
+        <v>512</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>202</v>
+      </c>
+      <c r="B26" s="20">
+        <v>513</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>202</v>
+      </c>
+      <c r="B27" s="20">
+        <v>514</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>194</v>
+      </c>
+      <c r="B28" s="20">
+        <v>515</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>202</v>
+      </c>
+      <c r="B29" s="20">
+        <v>520</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>202</v>
+      </c>
+      <c r="B30" s="20">
+        <v>1812</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>202</v>
+      </c>
+      <c r="B31" s="20">
+        <v>1813</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>194</v>
+      </c>
+      <c r="B32" s="20">
+        <v>2049</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>202</v>
+      </c>
+      <c r="B33" s="20">
+        <v>2049</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>194</v>
+      </c>
+      <c r="B34" s="20">
+        <v>2401</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>194</v>
+      </c>
+      <c r="B35" s="20">
+        <v>646</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>202</v>
+      </c>
+      <c r="B36" s="20">
+        <v>646</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>202</v>
+      </c>
+      <c r="B37" s="20">
+        <v>500</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>202</v>
+      </c>
+      <c r="B38" s="20">
+        <v>19</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>202</v>
+      </c>
+      <c r="B39" s="20">
+        <v>67</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>202</v>
+      </c>
+      <c r="B40" s="20">
+        <v>9</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>202</v>
+      </c>
+      <c r="B41" s="20">
+        <v>53</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>194</v>
+      </c>
+      <c r="B42" s="20">
+        <v>53</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>202</v>
+      </c>
+      <c r="B43" s="20">
+        <v>7</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>194</v>
+      </c>
+      <c r="B44" s="20">
+        <v>70</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>194</v>
+      </c>
+      <c r="B45" s="20">
+        <v>389</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>202</v>
+      </c>
+      <c r="B46" s="20">
+        <v>4500</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>202</v>
+      </c>
+      <c r="B47" s="20">
+        <v>1701</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>194</v>
+      </c>
+      <c r="B48" s="20">
+        <v>515</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>194</v>
+      </c>
+      <c r="B49" s="20">
+        <v>25</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>194</v>
+      </c>
+      <c r="B50" s="20">
+        <v>1863</v>
+      </c>
+      <c r="C50" s="20" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>194</v>
+      </c>
+      <c r="B51" s="20">
+        <v>1433</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>202</v>
+      </c>
+      <c r="B52" s="20">
+        <v>137</v>
+      </c>
+      <c r="C52" s="20" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>202</v>
+      </c>
+      <c r="B53" s="20">
+        <v>138</v>
+      </c>
+      <c r="C53" s="20" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>202</v>
+      </c>
+      <c r="B54" s="20">
+        <v>111</v>
+      </c>
+      <c r="C54" s="20" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>202</v>
+      </c>
+      <c r="B55" s="20">
+        <v>69</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>202</v>
+      </c>
+      <c r="B56" s="20">
+        <v>5632</v>
+      </c>
+      <c r="C56" s="20" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>202</v>
+      </c>
+      <c r="B57" s="20">
+        <v>1434</v>
+      </c>
+      <c r="C57" s="20" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>194</v>
+      </c>
+      <c r="B58" s="20">
+        <v>1525</v>
+      </c>
+      <c r="C58" s="20" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>194</v>
+      </c>
+      <c r="B59" s="20">
+        <v>1521</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>194</v>
+      </c>
+      <c r="B60" s="20">
+        <v>587</v>
+      </c>
+      <c r="C60" s="20" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>194</v>
+      </c>
+      <c r="B61" s="20">
+        <v>465</v>
+      </c>
+      <c r="C61" s="20" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>194</v>
+      </c>
+      <c r="B62" s="20">
+        <v>3389</v>
+      </c>
+      <c r="C62" s="20" t="s">
+        <v>255</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A0D1656-EFB0-4FAF-9FF7-4E21CC481274}">
+  <sheetPr>
+    <tabColor rgb="FFFF7171"/>
+  </sheetPr>
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.5546875" customWidth="1"/>
+    <col min="3" max="3" width="53.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C3" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" t="s">
+        <v>178</v>
+      </c>
+      <c r="C11" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FFCCECFF"/>
   </sheetPr>
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="2.44140625" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="2.44140625" customWidth="1"/>
-    <col min="9" max="9" width="2.33203125" customWidth="1"/>
-    <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="14" max="14" width="17" customWidth="1"/>
-    <col min="15" max="15" width="39.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="B1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" t="s">
-        <v>46</v>
-      </c>
-      <c r="N1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="E1" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="16"/>
+      <c r="B2" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" t="s">
-        <v>70</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="18"/>
+      <c r="E3" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="16"/>
+      <c r="B4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="K3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N3" t="s">
-        <v>47</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="N4" t="s">
-        <v>48</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="18"/>
+      <c r="B6" s="19" t="s">
         <v>13</v>
-      </c>
-      <c r="N5" t="s">
-        <v>53</v>
-      </c>
-      <c r="O5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="N6" t="s">
-        <v>65</v>
-      </c>
-      <c r="O6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>33</v>
-      </c>
-      <c r="N7" t="s">
-        <v>49</v>
-      </c>
-      <c r="O7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>34</v>
-      </c>
-      <c r="N8" t="s">
-        <v>50</v>
-      </c>
-      <c r="O8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>35</v>
-      </c>
-      <c r="N9" t="s">
-        <v>66</v>
-      </c>
-      <c r="O9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="4">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
-    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet5">
     <tabColor theme="2" tint="-0.249977111117893"/>
@@ -2371,19 +3488,19 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2391,7 +3508,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -2399,7 +3516,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -2407,7 +3524,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -2415,12 +3532,12 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -2428,7 +3545,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -2436,7 +3553,7 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -2444,7 +3561,7 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -2452,17 +3569,17 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -2470,7 +3587,7 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -2478,7 +3595,7 @@
         <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -2486,4 +3603,86 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AF5221-51D1-4864-A25A-0E399DB24E81}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="47.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>189</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>263</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>270</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added fw config validation
</commit_message>
<xml_diff>
--- a/fw_rules_test_02.xlsx
+++ b/fw_rules_test_02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\fw-rule-manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F874A9-3D80-47FD-8607-DDF2D752FD1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF85DF43-2028-4B55-AA4A-9935210F4A5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="647" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1113,6 +1113,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -1120,7 +1127,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1185,13 +1192,6 @@
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2183,7 +2183,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2273,10 +2273,10 @@
         <v>273</v>
       </c>
       <c r="K2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -2425,7 +2425,7 @@
         <v>274</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L6" s="6" t="s">
         <v>8</v>
@@ -2510,40 +2510,40 @@
   </sheetData>
   <autoFilter ref="A1:L8" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="K2:K1048576">
-    <cfRule type="cellIs" dxfId="16" priority="4296" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4296" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="4297" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4297" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L8">
-    <cfRule type="cellIs" dxfId="14" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="31" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="32" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D8">
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="10" operator="equal">
       <formula>"any"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F8">
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
       <formula>"any"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J8">
-    <cfRule type="cellIs" dxfId="9" priority="4299" operator="equal">
-      <formula>"permit"</formula>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"deny"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"reject"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
-      <formula>"deny"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="4299" operator="equal">
+      <formula>"permit"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">

</xml_diff>

<commit_message>
fix to connect to juniper fw
</commit_message>
<xml_diff>
--- a/fw_rules_test_02.xlsx
+++ b/fw_rules_test_02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\fw-rule-manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC09FAF-DC95-444F-A2BB-C88C51CF67B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE88878E-3DFB-4593-B7CA-9BCB98A1F485}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="647" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2183,7 +2183,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2270,13 +2270,13 @@
         <v>50410</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added destination port list
</commit_message>
<xml_diff>
--- a/fw_rules_test_02.xlsx
+++ b/fw_rules_test_02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\fw-rule-manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639383FD-0DA2-4A47-A070-3576F31EBD0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF09BDE-2E5B-47A1-B7DD-4B593E7A8F0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="647" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="281">
   <si>
     <t>Source Network</t>
   </si>
@@ -877,6 +877,18 @@
   </si>
   <si>
     <t>#TODO</t>
+  </si>
+  <si>
+    <t>21, 44</t>
+  </si>
+  <si>
+    <t>443, 555-666</t>
+  </si>
+  <si>
+    <t>5389, 888, 23</t>
+  </si>
+  <si>
+    <t>376, 999</t>
   </si>
 </sst>
 </file>
@@ -1112,7 +1124,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="53">
+  <dxfs count="46">
     <dxf>
       <fill>
         <patternFill>
@@ -1252,63 +1264,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF851A05"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2004,7 +1959,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2087,8 +2042,8 @@
       <c r="H2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="10">
-        <v>50410</v>
+      <c r="I2" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>272</v>
@@ -2097,7 +2052,7 @@
         <v>5</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -2125,8 +2080,8 @@
       <c r="H3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="10">
-        <v>5389</v>
+      <c r="I3" s="10" t="s">
+        <v>279</v>
       </c>
       <c r="J3" s="10" t="s">
         <v>273</v>
@@ -2163,8 +2118,8 @@
       <c r="H4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="10">
-        <v>443</v>
+      <c r="I4" s="10" t="s">
+        <v>278</v>
       </c>
       <c r="J4" s="10" t="s">
         <v>272</v>
@@ -2239,8 +2194,8 @@
       <c r="H6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="10">
-        <v>21</v>
+      <c r="I6" s="10" t="s">
+        <v>277</v>
       </c>
       <c r="J6" s="10" t="s">
         <v>274</v>

</xml_diff>

<commit_message>
Added feature: destination port list
</commit_message>
<xml_diff>
--- a/fw_rules_test_02.xlsx
+++ b/fw_rules_test_02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\fw-rule-manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF09BDE-2E5B-47A1-B7DD-4B593E7A8F0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB1CA13-B72D-4E8C-A761-7D093CD585EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="647" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2052,7 +2052,7 @@
         <v>5</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Changed action from Active to Enable to avoid confusion
</commit_message>
<xml_diff>
--- a/fw_rules_test_02.xlsx
+++ b/fw_rules_test_02.xlsx
@@ -8,18 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\fw-rule-manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD5E5DB-2EC8-4E79-AEEB-44B83972C14A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006F38E4-A6AA-4A15-A7A8-F8A1291E54E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="647" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="647" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Traffic Flows" sheetId="2" r:id="rId1"/>
     <sheet name="Address Book" sheetId="5" r:id="rId2"/>
-    <sheet name="Standard Apps" sheetId="7" r:id="rId3"/>
-    <sheet name="Zones" sheetId="8" r:id="rId4"/>
-    <sheet name="Dropdown Fields" sheetId="4" r:id="rId5"/>
-    <sheet name="Instructions" sheetId="1" r:id="rId6"/>
-    <sheet name="Feedback" sheetId="6" r:id="rId7"/>
+    <sheet name="Zones" sheetId="8" r:id="rId3"/>
+    <sheet name="Dropdown Fields" sheetId="4" r:id="rId4"/>
+    <sheet name="Instructions" sheetId="1" r:id="rId5"/>
+    <sheet name="Feedback" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Traffic Flows'!$A$1:$L$8</definedName>
@@ -46,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="218">
   <si>
     <t>Source Network</t>
   </si>
@@ -189,9 +188,6 @@
     <t>Source Port</t>
   </si>
   <si>
-    <t>Active</t>
-  </si>
-  <si>
     <t>Rule Name</t>
   </si>
   <si>
@@ -618,198 +614,6 @@
     <t>port ranges and list</t>
   </si>
   <si>
-    <t>tcp</t>
-  </si>
-  <si>
-    <t>junos-netbios-session</t>
-  </si>
-  <si>
-    <t>junos-smb-session</t>
-  </si>
-  <si>
-    <t>junos-ssh</t>
-  </si>
-  <si>
-    <t>junos-telnet</t>
-  </si>
-  <si>
-    <t>junos-smtp</t>
-  </si>
-  <si>
-    <t>junos-tacacs</t>
-  </si>
-  <si>
-    <t>junos-tacacs-ds</t>
-  </si>
-  <si>
-    <t>udp</t>
-  </si>
-  <si>
-    <t>junos-dhcp-client</t>
-  </si>
-  <si>
-    <t>junos-dhcp-server</t>
-  </si>
-  <si>
-    <t>junos-bootpc</t>
-  </si>
-  <si>
-    <t>junos-bootps</t>
-  </si>
-  <si>
-    <t>junos-finger</t>
-  </si>
-  <si>
-    <t>junos-http</t>
-  </si>
-  <si>
-    <t>junos-https</t>
-  </si>
-  <si>
-    <t>junos-pop3</t>
-  </si>
-  <si>
-    <t>junos-ident</t>
-  </si>
-  <si>
-    <t>junos-nntp</t>
-  </si>
-  <si>
-    <t>junos-ntp</t>
-  </si>
-  <si>
-    <t>junos-imap</t>
-  </si>
-  <si>
-    <t>junos-imaps</t>
-  </si>
-  <si>
-    <t>junos-bgp</t>
-  </si>
-  <si>
-    <t>junos-ldap</t>
-  </si>
-  <si>
-    <t>junos-snpp</t>
-  </si>
-  <si>
-    <t>junos-biff</t>
-  </si>
-  <si>
-    <t>junos-who</t>
-  </si>
-  <si>
-    <t>junos-syslog</t>
-  </si>
-  <si>
-    <t>junos-printer</t>
-  </si>
-  <si>
-    <t>junos-rip</t>
-  </si>
-  <si>
-    <t>junos-radius</t>
-  </si>
-  <si>
-    <t>junos-radacct</t>
-  </si>
-  <si>
-    <t>junos-nfsd-tcp</t>
-  </si>
-  <si>
-    <t>junos-nfsd-udp</t>
-  </si>
-  <si>
-    <t>junos-cvspserver</t>
-  </si>
-  <si>
-    <t>junos-ldp-tcp</t>
-  </si>
-  <si>
-    <t>junos-ldp-udp</t>
-  </si>
-  <si>
-    <t>junos-ike</t>
-  </si>
-  <si>
-    <t>junos-chargen</t>
-  </si>
-  <si>
-    <t>junos-dhcp-relay</t>
-  </si>
-  <si>
-    <t>junos-discard</t>
-  </si>
-  <si>
-    <t>junos-dns-udp</t>
-  </si>
-  <si>
-    <t>junos-dns-tcp</t>
-  </si>
-  <si>
-    <t>junos-echo</t>
-  </si>
-  <si>
-    <t>junos-gopher</t>
-  </si>
-  <si>
-    <t>junos-internet-locator-service</t>
-  </si>
-  <si>
-    <t>junos-ike-nat</t>
-  </si>
-  <si>
-    <t>junos-l2tp</t>
-  </si>
-  <si>
-    <t>junos-lpr</t>
-  </si>
-  <si>
-    <t>junos-mail</t>
-  </si>
-  <si>
-    <t>junos-msn</t>
-  </si>
-  <si>
-    <t>junos-ms-sql</t>
-  </si>
-  <si>
-    <t>junos-nbname</t>
-  </si>
-  <si>
-    <t>junos-nbds</t>
-  </si>
-  <si>
-    <t>junos-nfs</t>
-  </si>
-  <si>
-    <t>junos-nsm</t>
-  </si>
-  <si>
-    <t>junos-pc-anywhere</t>
-  </si>
-  <si>
-    <t>junos-sql-monitor</t>
-  </si>
-  <si>
-    <t>junos-sqlnet-v1</t>
-  </si>
-  <si>
-    <t>junos-sqlnet-v2</t>
-  </si>
-  <si>
-    <t>junos-smtps</t>
-  </si>
-  <si>
-    <t>junos-rdp</t>
-  </si>
-  <si>
-    <t>JUNOS-Name</t>
-  </si>
-  <si>
-    <t>Port</t>
-  </si>
-  <si>
     <t>globansible01.esbu.local</t>
   </si>
   <si>
@@ -834,6 +638,9 @@
     <t>Zone Set</t>
   </si>
   <si>
+    <t>internal1, internal2</t>
+  </si>
+  <si>
     <t>dmz1, dmz2, internal1, internal2, servers1, internet-untrust</t>
   </si>
   <si>
@@ -882,13 +689,16 @@
     <t>5389, 888, 23</t>
   </si>
   <si>
-    <t>376, 999</t>
-  </si>
-  <si>
     <t>review process ?</t>
   </si>
   <si>
-    <t>internal1, internal2, zone-xxx</t>
+    <t>globansible01, azure-host-10.248.56.200</t>
+  </si>
+  <si>
+    <t>application-objects - groups , protocol - app-group</t>
+  </si>
+  <si>
+    <t>Enable</t>
   </si>
 </sst>
 </file>
@@ -1130,16 +940,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="46">
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -1158,305 +968,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF851A05"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1972,9 +1483,9 @@
   </sheetPr>
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1986,7 +1497,7 @@
     <col min="5" max="5" width="44.6640625" style="8" customWidth="1"/>
     <col min="6" max="6" width="22.6640625" style="11" customWidth="1"/>
     <col min="7" max="7" width="28.6640625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="10" style="8" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" style="8" customWidth="1"/>
     <col min="9" max="9" width="14" style="11" customWidth="1"/>
     <col min="10" max="10" width="10.33203125" style="11" customWidth="1"/>
     <col min="11" max="11" width="9" style="8" customWidth="1"/>
@@ -1996,7 +1507,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
@@ -2023,10 +1534,10 @@
         <v>3</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>268</v>
+        <v>204</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>47</v>
+        <v>217</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>45</v>
@@ -2037,31 +1548,31 @@
         <v>26</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>266</v>
+        <v>202</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="10" t="s">
-        <v>278</v>
+      <c r="I2" s="23">
+        <v>389</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>270</v>
+        <v>206</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>5</v>
@@ -2087,19 +1598,19 @@
         <v>12</v>
       </c>
       <c r="F3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>52</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>9</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>277</v>
+        <v>213</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>270</v>
+        <v>208</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>5</v>
@@ -2119,25 +1630,25 @@
         <v>12</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>266</v>
+        <v>202</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>266</v>
+        <v>202</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>276</v>
+        <v>212</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>270</v>
+        <v>206</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>5</v>
@@ -2157,16 +1668,16 @@
         <v>12</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>267</v>
+        <v>203</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>33</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>9</v>
@@ -2175,7 +1686,7 @@
         <v>443</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>270</v>
+        <v>206</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>5</v>
@@ -2186,19 +1697,19 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>180</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>181</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>96</v>
+        <v>215</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>38</v>
@@ -2210,10 +1721,10 @@
         <v>9</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>275</v>
+        <v>211</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>272</v>
+        <v>207</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>5</v>
@@ -2224,22 +1735,22 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>56</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>12</v>
@@ -2251,7 +1762,7 @@
         <v>22</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>270</v>
+        <v>206</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>5</v>
@@ -2262,22 +1773,22 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>12</v>
@@ -2289,7 +1800,7 @@
         <v>22</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>270</v>
+        <v>206</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>5</v>
@@ -2385,7 +1896,7 @@
   <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2397,10 +1908,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>4</v>
@@ -2408,467 +1919,467 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>255</v>
+        <v>190</v>
       </c>
       <c r="C2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
         <v>59</v>
-      </c>
-      <c r="B3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
         <v>61</v>
       </c>
-      <c r="B4" t="s">
-        <v>62</v>
-      </c>
       <c r="C4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
         <v>63</v>
       </c>
-      <c r="B5" t="s">
-        <v>64</v>
-      </c>
       <c r="C5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
         <v>65</v>
-      </c>
-      <c r="B6" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>256</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" t="s">
         <v>68</v>
-      </c>
-      <c r="B8" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" t="s">
         <v>70</v>
-      </c>
-      <c r="B9" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
-        <v>257</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>258</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" t="s">
         <v>74</v>
-      </c>
-      <c r="B12" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" t="s">
         <v>76</v>
-      </c>
-      <c r="B13" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" t="s">
         <v>78</v>
-      </c>
-      <c r="B14" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" t="s">
         <v>80</v>
-      </c>
-      <c r="B15" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" t="s">
         <v>82</v>
-      </c>
-      <c r="B16" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" t="s">
         <v>84</v>
-      </c>
-      <c r="B17" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" t="s">
         <v>86</v>
-      </c>
-      <c r="B18" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" t="s">
         <v>88</v>
-      </c>
-      <c r="B19" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" t="s">
         <v>90</v>
-      </c>
-      <c r="B20" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" t="s">
         <v>92</v>
-      </c>
-      <c r="B21" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" t="s">
         <v>94</v>
-      </c>
-      <c r="B22" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B23" t="s">
-        <v>254</v>
+        <v>189</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" t="s">
         <v>97</v>
-      </c>
-      <c r="B24" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" t="s">
         <v>99</v>
-      </c>
-      <c r="B25" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26" t="s">
         <v>101</v>
-      </c>
-      <c r="B26" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>102</v>
+      </c>
+      <c r="B27" t="s">
         <v>103</v>
-      </c>
-      <c r="B27" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>104</v>
+      </c>
+      <c r="B28" t="s">
         <v>105</v>
-      </c>
-      <c r="B28" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" t="s">
         <v>107</v>
-      </c>
-      <c r="B29" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>108</v>
+      </c>
+      <c r="B30" t="s">
         <v>109</v>
-      </c>
-      <c r="B30" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" t="s">
         <v>111</v>
-      </c>
-      <c r="B31" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>112</v>
+      </c>
+      <c r="B32" t="s">
         <v>113</v>
-      </c>
-      <c r="B32" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>114</v>
+      </c>
+      <c r="B33" t="s">
         <v>115</v>
-      </c>
-      <c r="B33" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>116</v>
+      </c>
+      <c r="B34" t="s">
         <v>117</v>
-      </c>
-      <c r="B34" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>118</v>
+      </c>
+      <c r="B35" t="s">
         <v>119</v>
-      </c>
-      <c r="B35" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>120</v>
+      </c>
+      <c r="B36" t="s">
         <v>121</v>
-      </c>
-      <c r="B36" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>122</v>
+      </c>
+      <c r="B37" t="s">
         <v>123</v>
-      </c>
-      <c r="B37" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>124</v>
+      </c>
+      <c r="B38" t="s">
         <v>125</v>
-      </c>
-      <c r="B38" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>126</v>
+      </c>
+      <c r="B39" t="s">
         <v>127</v>
-      </c>
-      <c r="B39" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>128</v>
+      </c>
+      <c r="B40" t="s">
         <v>129</v>
-      </c>
-      <c r="B40" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>130</v>
+      </c>
+      <c r="B41" t="s">
         <v>131</v>
-      </c>
-      <c r="B41" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>132</v>
+      </c>
+      <c r="B42" t="s">
         <v>133</v>
-      </c>
-      <c r="B42" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>134</v>
+      </c>
+      <c r="B43" t="s">
         <v>135</v>
-      </c>
-      <c r="B43" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>136</v>
+      </c>
+      <c r="B44" t="s">
         <v>137</v>
-      </c>
-      <c r="B44" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>138</v>
+      </c>
+      <c r="B45" t="s">
         <v>139</v>
-      </c>
-      <c r="B45" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>140</v>
+      </c>
+      <c r="B46" t="s">
         <v>141</v>
-      </c>
-      <c r="B46" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>142</v>
+      </c>
+      <c r="B47" t="s">
         <v>143</v>
-      </c>
-      <c r="B47" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>144</v>
+      </c>
+      <c r="B48" t="s">
         <v>145</v>
-      </c>
-      <c r="B48" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>146</v>
+      </c>
+      <c r="B49" t="s">
         <v>147</v>
-      </c>
-      <c r="B49" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>148</v>
+      </c>
+      <c r="B50" t="s">
         <v>149</v>
-      </c>
-      <c r="B50" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>150</v>
+      </c>
+      <c r="B51" t="s">
         <v>151</v>
-      </c>
-      <c r="B51" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>152</v>
+      </c>
+      <c r="B52" t="s">
         <v>153</v>
-      </c>
-      <c r="B52" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B53" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>155</v>
+      </c>
+      <c r="B54" t="s">
         <v>156</v>
-      </c>
-      <c r="B54" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>157</v>
+      </c>
+      <c r="B55" t="s">
         <v>158</v>
-      </c>
-      <c r="B55" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>159</v>
+      </c>
+      <c r="B56" t="s">
         <v>160</v>
-      </c>
-      <c r="B56" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>161</v>
+      </c>
+      <c r="B57" t="s">
         <v>162</v>
-      </c>
-      <c r="B57" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
+        <v>163</v>
+      </c>
+      <c r="B58" t="s">
         <v>164</v>
-      </c>
-      <c r="B58" t="s">
-        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -2878,718 +2389,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7C7E070-0DF1-46AD-B71D-FFAED45E81B9}">
-  <sheetPr>
-    <tabColor rgb="FFFFCC00"/>
-  </sheetPr>
-  <dimension ref="A1:C62"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" customWidth="1"/>
-    <col min="4" max="4" width="18.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B2" s="21">
-        <v>139</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B3" s="21">
-        <v>445</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>190</v>
-      </c>
-      <c r="B4" s="21">
-        <v>22</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>190</v>
-      </c>
-      <c r="B5" s="21">
-        <v>23</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>190</v>
-      </c>
-      <c r="B6" s="21">
-        <v>25</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>190</v>
-      </c>
-      <c r="B7" s="21">
-        <v>49</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>190</v>
-      </c>
-      <c r="B8" s="21">
-        <v>65</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>198</v>
-      </c>
-      <c r="B9" s="21">
-        <v>68</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>198</v>
-      </c>
-      <c r="B10" s="21">
-        <v>67</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>198</v>
-      </c>
-      <c r="B11" s="21">
-        <v>68</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>198</v>
-      </c>
-      <c r="B12" s="21">
-        <v>67</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>190</v>
-      </c>
-      <c r="B13" s="21">
-        <v>79</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>190</v>
-      </c>
-      <c r="B14" s="21">
-        <v>80</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>190</v>
-      </c>
-      <c r="B15" s="21">
-        <v>443</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>190</v>
-      </c>
-      <c r="B16" s="21">
-        <v>110</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>190</v>
-      </c>
-      <c r="B17" s="21">
-        <v>113</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>190</v>
-      </c>
-      <c r="B18" s="21">
-        <v>119</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>198</v>
-      </c>
-      <c r="B19" s="21">
-        <v>123</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>190</v>
-      </c>
-      <c r="B20" s="21">
-        <v>143</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>190</v>
-      </c>
-      <c r="B21" s="21">
-        <v>993</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>190</v>
-      </c>
-      <c r="B22" s="21">
-        <v>179</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>190</v>
-      </c>
-      <c r="B23" s="21">
-        <v>389</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>190</v>
-      </c>
-      <c r="B24" s="21">
-        <v>444</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>198</v>
-      </c>
-      <c r="B25" s="21">
-        <v>512</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>198</v>
-      </c>
-      <c r="B26" s="21">
-        <v>513</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>198</v>
-      </c>
-      <c r="B27" s="21">
-        <v>514</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>190</v>
-      </c>
-      <c r="B28" s="21">
-        <v>515</v>
-      </c>
-      <c r="C28" s="21" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>198</v>
-      </c>
-      <c r="B29" s="21">
-        <v>520</v>
-      </c>
-      <c r="C29" s="21" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>198</v>
-      </c>
-      <c r="B30" s="21">
-        <v>1812</v>
-      </c>
-      <c r="C30" s="21" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>198</v>
-      </c>
-      <c r="B31" s="21">
-        <v>1813</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>190</v>
-      </c>
-      <c r="B32" s="21">
-        <v>2049</v>
-      </c>
-      <c r="C32" s="21" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>198</v>
-      </c>
-      <c r="B33" s="21">
-        <v>2049</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>190</v>
-      </c>
-      <c r="B34" s="21">
-        <v>2401</v>
-      </c>
-      <c r="C34" s="21" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>190</v>
-      </c>
-      <c r="B35" s="21">
-        <v>646</v>
-      </c>
-      <c r="C35" s="21" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>198</v>
-      </c>
-      <c r="B36" s="21">
-        <v>646</v>
-      </c>
-      <c r="C36" s="21" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>198</v>
-      </c>
-      <c r="B37" s="21">
-        <v>500</v>
-      </c>
-      <c r="C37" s="21" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>198</v>
-      </c>
-      <c r="B38" s="21">
-        <v>19</v>
-      </c>
-      <c r="C38" s="21" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>198</v>
-      </c>
-      <c r="B39" s="21">
-        <v>67</v>
-      </c>
-      <c r="C39" s="21" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>198</v>
-      </c>
-      <c r="B40" s="21">
-        <v>9</v>
-      </c>
-      <c r="C40" s="21" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>198</v>
-      </c>
-      <c r="B41" s="21">
-        <v>53</v>
-      </c>
-      <c r="C41" s="21" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>190</v>
-      </c>
-      <c r="B42" s="21">
-        <v>53</v>
-      </c>
-      <c r="C42" s="21" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>198</v>
-      </c>
-      <c r="B43" s="21">
-        <v>7</v>
-      </c>
-      <c r="C43" s="21" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>190</v>
-      </c>
-      <c r="B44" s="21">
-        <v>70</v>
-      </c>
-      <c r="C44" s="21" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>190</v>
-      </c>
-      <c r="B45" s="21">
-        <v>389</v>
-      </c>
-      <c r="C45" s="21" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>198</v>
-      </c>
-      <c r="B46" s="21">
-        <v>4500</v>
-      </c>
-      <c r="C46" s="21" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>198</v>
-      </c>
-      <c r="B47" s="21">
-        <v>1701</v>
-      </c>
-      <c r="C47" s="21" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>190</v>
-      </c>
-      <c r="B48" s="21">
-        <v>515</v>
-      </c>
-      <c r="C48" s="21" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>190</v>
-      </c>
-      <c r="B49" s="21">
-        <v>25</v>
-      </c>
-      <c r="C49" s="21" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>190</v>
-      </c>
-      <c r="B50" s="21">
-        <v>1863</v>
-      </c>
-      <c r="C50" s="21" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>190</v>
-      </c>
-      <c r="B51" s="21">
-        <v>1433</v>
-      </c>
-      <c r="C51" s="21" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>198</v>
-      </c>
-      <c r="B52" s="21">
-        <v>137</v>
-      </c>
-      <c r="C52" s="21" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>198</v>
-      </c>
-      <c r="B53" s="21">
-        <v>138</v>
-      </c>
-      <c r="C53" s="21" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>198</v>
-      </c>
-      <c r="B54" s="21">
-        <v>111</v>
-      </c>
-      <c r="C54" s="21" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>198</v>
-      </c>
-      <c r="B55" s="21">
-        <v>69</v>
-      </c>
-      <c r="C55" s="21" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>198</v>
-      </c>
-      <c r="B56" s="21">
-        <v>5632</v>
-      </c>
-      <c r="C56" s="21" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>198</v>
-      </c>
-      <c r="B57" s="21">
-        <v>1434</v>
-      </c>
-      <c r="C57" s="21" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>190</v>
-      </c>
-      <c r="B58" s="21">
-        <v>1525</v>
-      </c>
-      <c r="C58" s="21" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>190</v>
-      </c>
-      <c r="B59" s="21">
-        <v>1521</v>
-      </c>
-      <c r="C59" s="21" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>190</v>
-      </c>
-      <c r="B60" s="21">
-        <v>587</v>
-      </c>
-      <c r="C60" s="21" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>190</v>
-      </c>
-      <c r="B61" s="21">
-        <v>465</v>
-      </c>
-      <c r="C61" s="21" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>190</v>
-      </c>
-      <c r="B62" s="21">
-        <v>3389</v>
-      </c>
-      <c r="C62" s="21" t="s">
-        <v>251</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A0D1656-EFB0-4FAF-9FF7-4E21CC481274}">
   <sheetPr>
     <tabColor rgb="FFFF7171"/>
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -3602,10 +2408,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>260</v>
+        <v>195</v>
       </c>
       <c r="B1" t="s">
-        <v>261</v>
+        <v>196</v>
       </c>
       <c r="C1" t="s">
         <v>27</v>
@@ -3613,24 +2419,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>266</v>
+        <v>202</v>
       </c>
       <c r="B2" t="s">
-        <v>262</v>
+        <v>198</v>
       </c>
       <c r="C2" t="s">
-        <v>263</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>267</v>
+        <v>203</v>
       </c>
       <c r="B3" t="s">
-        <v>280</v>
+        <v>197</v>
       </c>
       <c r="C3" t="s">
-        <v>264</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3668,10 +2474,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
         <v>40</v>
@@ -3701,10 +2507,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>36</v>
@@ -3712,27 +2518,28 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>175</v>
+      </c>
+      <c r="B11" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" t="s">
         <v>176</v>
-      </c>
-      <c r="B11" t="s">
-        <v>176</v>
-      </c>
-      <c r="C11" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="bLmCN/AYSoW/dCMN7Q6HdVlZT7wUuTZsRVUBF+wyXRx05oBvQYK+kyOoTjqUU23ySIGMMvcQoDtc2qXzw5CenQ==" saltValue="sU0vsq250vQEjxowBGvmuA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3741,7 +2548,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FFCCECFF"/>
@@ -3749,7 +2556,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3768,19 +2575,19 @@
         <v>2</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>269</v>
+        <v>205</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>269</v>
+        <v>205</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>268</v>
+        <v>204</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>269</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -3794,7 +2601,7 @@
       </c>
       <c r="G2" s="16"/>
       <c r="H2" s="17" t="s">
-        <v>270</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3808,7 +2615,7 @@
       </c>
       <c r="G3" s="16"/>
       <c r="H3" s="17" t="s">
-        <v>271</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3818,10 +2625,11 @@
       </c>
       <c r="G4" s="18"/>
       <c r="H4" s="19" t="s">
-        <v>272</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="2egXIuU8MC/uBPq9LD/l2KGbvWr/R96EIj4NJCfJ3AVlGxfchsvQ7CD+tvCD1GnWrIOC1ZrzGdJWUGI99vkjhg==" saltValue="4080Anc2sLS20VUJe4D8GQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3833,14 +2641,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet5">
     <tabColor theme="2" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -3922,7 +2730,7 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -3952,15 +2760,16 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="PCugRULIkoJFfOFVo//wMwEXv3pQvwEGLyLWhWDhedoiHtH24X8PSZrS2oCqC+32lmNoDHyxrT+D/0k4PdY7Ow==" saltValue="HLjKgnGaRnKSBF1AGjxcvA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AF5221-51D1-4864-A25A-0E399DB24E81}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
@@ -3974,90 +2783,98 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>265</v>
+        <v>181</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>274</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B3" t="s">
-        <v>274</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>279</v>
+        <v>214</v>
       </c>
       <c r="B4" t="s">
-        <v>274</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>273</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>265</v>
+        <v>209</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>188</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>265</v>
+        <v>187</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>189</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>265</v>
+        <v>188</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>185</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>265</v>
+        <v>184</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>186</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>265</v>
+        <v>185</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B10" t="s">
-        <v>274</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>259</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>265</v>
+        <v>194</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>216</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added CLI options, added feature to use named applications, moved network handlers into a new file
</commit_message>
<xml_diff>
--- a/fw_rules_test_02.xlsx
+++ b/fw_rules_test_02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\fw-rule-manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006F38E4-A6AA-4A15-A7A8-F8A1291E54E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B55B31-0309-4409-A5A6-A917FA46777F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="647" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,9 +16,10 @@
     <sheet name="Traffic Flows" sheetId="2" r:id="rId1"/>
     <sheet name="Address Book" sheetId="5" r:id="rId2"/>
     <sheet name="Zones" sheetId="8" r:id="rId3"/>
-    <sheet name="Dropdown Fields" sheetId="4" r:id="rId4"/>
-    <sheet name="Instructions" sheetId="1" r:id="rId5"/>
-    <sheet name="Feedback" sheetId="6" r:id="rId6"/>
+    <sheet name="Applications" sheetId="9" r:id="rId4"/>
+    <sheet name="Dropdown Fields" sheetId="4" r:id="rId5"/>
+    <sheet name="Instructions" sheetId="1" r:id="rId6"/>
+    <sheet name="Feedback" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Traffic Flows'!$A$1:$L$8</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="266">
   <si>
     <t>Source Network</t>
   </si>
@@ -614,6 +615,15 @@
     <t>port ranges and list</t>
   </si>
   <si>
+    <t>tcp</t>
+  </si>
+  <si>
+    <t>udp</t>
+  </si>
+  <si>
+    <t>Port</t>
+  </si>
+  <si>
     <t>globansible01.esbu.local</t>
   </si>
   <si>
@@ -686,9 +696,6 @@
     <t>443, 555-666</t>
   </si>
   <si>
-    <t>5389, 888, 23</t>
-  </si>
-  <si>
     <t>review process ?</t>
   </si>
   <si>
@@ -699,6 +706,144 @@
   </si>
   <si>
     <t>Enable</t>
+  </si>
+  <si>
+    <t>tftp</t>
+  </si>
+  <si>
+    <t>netbios-session</t>
+  </si>
+  <si>
+    <t>smb-session</t>
+  </si>
+  <si>
+    <t>ssh</t>
+  </si>
+  <si>
+    <t>telnet</t>
+  </si>
+  <si>
+    <t>smtp</t>
+  </si>
+  <si>
+    <t>tacacs</t>
+  </si>
+  <si>
+    <t>tacacs-ds</t>
+  </si>
+  <si>
+    <t>dhcp-client</t>
+  </si>
+  <si>
+    <t>dhcp-server</t>
+  </si>
+  <si>
+    <t>bootpc</t>
+  </si>
+  <si>
+    <t>bootps</t>
+  </si>
+  <si>
+    <t>finger</t>
+  </si>
+  <si>
+    <t>http</t>
+  </si>
+  <si>
+    <t>https</t>
+  </si>
+  <si>
+    <t>pop3</t>
+  </si>
+  <si>
+    <t>ntp</t>
+  </si>
+  <si>
+    <t>imap</t>
+  </si>
+  <si>
+    <t>imaps</t>
+  </si>
+  <si>
+    <t>bgp</t>
+  </si>
+  <si>
+    <t>ldap</t>
+  </si>
+  <si>
+    <t>snpp</t>
+  </si>
+  <si>
+    <t>syslog</t>
+  </si>
+  <si>
+    <t>radius</t>
+  </si>
+  <si>
+    <t>radacct</t>
+  </si>
+  <si>
+    <t>nfsd-tcp</t>
+  </si>
+  <si>
+    <t>nfsd-udp</t>
+  </si>
+  <si>
+    <t>cvspserver</t>
+  </si>
+  <si>
+    <t>ldp-tcp</t>
+  </si>
+  <si>
+    <t>ldp-udp</t>
+  </si>
+  <si>
+    <t>ike</t>
+  </si>
+  <si>
+    <t>dns-udp</t>
+  </si>
+  <si>
+    <t>dns-tcp</t>
+  </si>
+  <si>
+    <t>ike-nat</t>
+  </si>
+  <si>
+    <t>mail</t>
+  </si>
+  <si>
+    <t>ms-sql</t>
+  </si>
+  <si>
+    <t>nbname</t>
+  </si>
+  <si>
+    <t>nbds</t>
+  </si>
+  <si>
+    <t>nfs</t>
+  </si>
+  <si>
+    <t>sql-monitor</t>
+  </si>
+  <si>
+    <t>sqlnet-v1</t>
+  </si>
+  <si>
+    <t>rdp</t>
+  </si>
+  <si>
+    <t>smtps-t1</t>
+  </si>
+  <si>
+    <t>smtps-t2</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>https, http, ssh</t>
   </si>
 </sst>
 </file>
@@ -794,7 +939,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -824,6 +969,19 @@
       <right style="thin">
         <color theme="4" tint="0.39997558519241921"/>
       </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
       <top style="thin">
         <color theme="4" tint="0.39997558519241921"/>
       </top>
@@ -898,7 +1056,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -933,12 +1091,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1025,11 +1184,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCCECFF"/>
       <color rgb="FF851A05"/>
       <color rgb="FF33CC33"/>
       <color rgb="FFFF7171"/>
       <color rgb="FFFFCC00"/>
-      <color rgb="FFCCECFF"/>
       <color rgb="FF3379CD"/>
       <color rgb="FF006600"/>
       <color rgb="FF89B0FF"/>
@@ -1485,7 +1644,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1534,10 +1693,10 @@
         <v>3</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>45</v>
@@ -1554,7 +1713,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>178</v>
@@ -1568,11 +1727,11 @@
       <c r="H2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="23">
-        <v>389</v>
+      <c r="I2" s="24" t="s">
+        <v>239</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>5</v>
@@ -1607,10 +1766,10 @@
         <v>9</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>213</v>
+        <v>265</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>5</v>
@@ -1630,13 +1789,13 @@
         <v>12</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>177</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>56</v>
@@ -1645,10 +1804,10 @@
         <v>9</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>5</v>
@@ -1668,7 +1827,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>177</v>
@@ -1686,7 +1845,7 @@
         <v>443</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>5</v>
@@ -1709,7 +1868,7 @@
         <v>49</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>38</v>
@@ -1721,10 +1880,10 @@
         <v>9</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>5</v>
@@ -1758,11 +1917,11 @@
       <c r="H7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="10">
-        <v>22</v>
+      <c r="I7" s="10" t="s">
+        <v>223</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>5</v>
@@ -1800,7 +1959,7 @@
         <v>22</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>5</v>
@@ -1922,7 +2081,7 @@
         <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C2" t="s">
         <v>166</v>
@@ -1971,7 +2130,7 @@
         <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1995,7 +2154,7 @@
         <v>71</v>
       </c>
       <c r="B10" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -2003,7 +2162,7 @@
         <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -2099,7 +2258,7 @@
         <v>95</v>
       </c>
       <c r="B23" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -2395,9 +2554,7 @@
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2408,10 +2565,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C1" t="s">
         <v>27</v>
@@ -2419,24 +2576,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C2" t="s">
         <v>202</v>
-      </c>
-      <c r="B2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C3" t="s">
         <v>203</v>
-      </c>
-      <c r="B3" t="s">
-        <v>197</v>
-      </c>
-      <c r="C3" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2539,7 +2696,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="bLmCN/AYSoW/dCMN7Q6HdVlZT7wUuTZsRVUBF+wyXRx05oBvQYK+kyOoTjqUU23ySIGMMvcQoDtc2qXzw5CenQ==" saltValue="sU0vsq250vQEjxowBGvmuA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2549,6 +2706,527 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A34D0642-76C8-4CC6-885F-4BF860F6DBDF}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:C45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C5">
+        <v>2401</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>229</v>
+      </c>
+      <c r="B7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C7">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C8">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>251</v>
+      </c>
+      <c r="B9" t="s">
+        <v>190</v>
+      </c>
+      <c r="C9">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>232</v>
+      </c>
+      <c r="B10" t="s">
+        <v>189</v>
+      </c>
+      <c r="C10">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>233</v>
+      </c>
+      <c r="B11" t="s">
+        <v>189</v>
+      </c>
+      <c r="C11">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>234</v>
+      </c>
+      <c r="B12" t="s">
+        <v>189</v>
+      </c>
+      <c r="C12">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>250</v>
+      </c>
+      <c r="B13" t="s">
+        <v>190</v>
+      </c>
+      <c r="C13">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>253</v>
+      </c>
+      <c r="B14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C14">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>237</v>
+      </c>
+      <c r="B15" t="s">
+        <v>189</v>
+      </c>
+      <c r="C15">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>238</v>
+      </c>
+      <c r="B16" t="s">
+        <v>189</v>
+      </c>
+      <c r="C16">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>240</v>
+      </c>
+      <c r="B17" t="s">
+        <v>189</v>
+      </c>
+      <c r="C17">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>248</v>
+      </c>
+      <c r="B18" t="s">
+        <v>189</v>
+      </c>
+      <c r="C18">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>249</v>
+      </c>
+      <c r="B19" t="s">
+        <v>190</v>
+      </c>
+      <c r="C19">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>254</v>
+      </c>
+      <c r="B20" t="s">
+        <v>189</v>
+      </c>
+      <c r="C20">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>255</v>
+      </c>
+      <c r="B21" t="s">
+        <v>189</v>
+      </c>
+      <c r="C21">
+        <v>1433</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>257</v>
+      </c>
+      <c r="B22" t="s">
+        <v>190</v>
+      </c>
+      <c r="C22">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>256</v>
+      </c>
+      <c r="B23" t="s">
+        <v>190</v>
+      </c>
+      <c r="C23">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>221</v>
+      </c>
+      <c r="B24" t="s">
+        <v>189</v>
+      </c>
+      <c r="C24">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>258</v>
+      </c>
+      <c r="B25" t="s">
+        <v>190</v>
+      </c>
+      <c r="C25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>245</v>
+      </c>
+      <c r="B26" t="s">
+        <v>189</v>
+      </c>
+      <c r="C26">
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>246</v>
+      </c>
+      <c r="B27" t="s">
+        <v>190</v>
+      </c>
+      <c r="C27">
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>236</v>
+      </c>
+      <c r="B28" t="s">
+        <v>190</v>
+      </c>
+      <c r="C28">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>235</v>
+      </c>
+      <c r="B29" t="s">
+        <v>189</v>
+      </c>
+      <c r="C29">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>244</v>
+      </c>
+      <c r="B30" t="s">
+        <v>190</v>
+      </c>
+      <c r="C30">
+        <v>1813</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>243</v>
+      </c>
+      <c r="B31" t="s">
+        <v>190</v>
+      </c>
+      <c r="C31">
+        <v>1812</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>261</v>
+      </c>
+      <c r="B32" t="s">
+        <v>189</v>
+      </c>
+      <c r="C32">
+        <v>3389</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>222</v>
+      </c>
+      <c r="B33" t="s">
+        <v>189</v>
+      </c>
+      <c r="C33">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>225</v>
+      </c>
+      <c r="B34" t="s">
+        <v>189</v>
+      </c>
+      <c r="C34">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>262</v>
+      </c>
+      <c r="B35" t="s">
+        <v>189</v>
+      </c>
+      <c r="C35">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>263</v>
+      </c>
+      <c r="B36" t="s">
+        <v>189</v>
+      </c>
+      <c r="C36">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>241</v>
+      </c>
+      <c r="B37" t="s">
+        <v>189</v>
+      </c>
+      <c r="C37">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>259</v>
+      </c>
+      <c r="B38" t="s">
+        <v>190</v>
+      </c>
+      <c r="C38">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>260</v>
+      </c>
+      <c r="B39" t="s">
+        <v>189</v>
+      </c>
+      <c r="C39">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>223</v>
+      </c>
+      <c r="B40" t="s">
+        <v>189</v>
+      </c>
+      <c r="C40">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>242</v>
+      </c>
+      <c r="B41" t="s">
+        <v>190</v>
+      </c>
+      <c r="C41">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>226</v>
+      </c>
+      <c r="B42" t="s">
+        <v>189</v>
+      </c>
+      <c r="C42">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>227</v>
+      </c>
+      <c r="B43" t="s">
+        <v>189</v>
+      </c>
+      <c r="C43">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>224</v>
+      </c>
+      <c r="B44" t="s">
+        <v>189</v>
+      </c>
+      <c r="C44">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>220</v>
+      </c>
+      <c r="B45" t="s">
+        <v>190</v>
+      </c>
+      <c r="C45">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C61">
+    <sortCondition ref="A2:A61"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FFCCECFF"/>
@@ -2571,61 +3249,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="D1" s="14" t="s">
+      <c r="B1" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>204</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>205</v>
+      <c r="E1" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="17" t="s">
+      <c r="A2" s="17"/>
+      <c r="B2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17" t="s">
+      <c r="D2" s="17"/>
+      <c r="E2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="17" t="s">
-        <v>206</v>
+      <c r="G2" s="17"/>
+      <c r="H2" s="18" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="16"/>
-      <c r="B3" s="17" t="s">
+      <c r="A3" s="17"/>
+      <c r="B3" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19" t="s">
+      <c r="D3" s="19"/>
+      <c r="E3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="17" t="s">
-        <v>207</v>
+      <c r="G3" s="17"/>
+      <c r="H3" s="18" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="19"/>
+      <c r="B4" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="19" t="s">
-        <v>208</v>
+      <c r="G4" s="19"/>
+      <c r="H4" s="20" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -2641,7 +3319,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet5">
     <tabColor theme="2" tint="-0.249977111117893"/>
@@ -2767,7 +3445,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AF5221-51D1-4864-A25A-0E399DB24E81}">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -2785,16 +3463,16 @@
       <c r="A1" t="s">
         <v>181</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>201</v>
+      <c r="B1" s="22" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>182</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>210</v>
+      <c r="B2" s="21" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2802,55 +3480,55 @@
         <v>183</v>
       </c>
       <c r="B3" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B4" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>209</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>201</v>
+        <v>212</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>187</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>201</v>
+      <c r="B6" s="23" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>188</v>
       </c>
-      <c r="B7" s="21" t="s">
-        <v>201</v>
+      <c r="B7" s="22" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>184</v>
       </c>
-      <c r="B8" s="21" t="s">
-        <v>201</v>
+      <c r="B8" s="22" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>185</v>
       </c>
-      <c r="B9" s="21" t="s">
-        <v>201</v>
+      <c r="B9" s="22" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -2858,23 +3536,23 @@
         <v>186</v>
       </c>
       <c r="B10" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>194</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>201</v>
+        <v>197</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>216</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>210</v>
+        <v>218</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved handling data into separate functions and modules
</commit_message>
<xml_diff>
--- a/fw_rules_test_02.xlsx
+++ b/fw_rules_test_02.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\fw-rule-manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B55B31-0309-4409-A5A6-A917FA46777F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9A0A31-061D-4B92-BB8C-85D4C240E089}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="647" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="647" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Traffic Flows" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="267">
   <si>
     <t>Source Network</t>
   </si>
@@ -844,6 +844,9 @@
   </si>
   <si>
     <t>https, http, ssh</t>
+  </si>
+  <si>
+    <t>443, smtp</t>
   </si>
 </sst>
 </file>
@@ -1644,7 +1647,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1841,8 +1844,8 @@
       <c r="H5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="10">
-        <v>443</v>
+      <c r="I5" s="10" t="s">
+        <v>266</v>
       </c>
       <c r="J5" s="10" t="s">
         <v>209</v>

</xml_diff>

<commit_message>
Added standard Network OS Apps lookup
</commit_message>
<xml_diff>
--- a/fw_rules_test_02.xlsx
+++ b/fw_rules_test_02.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\fw-rule-manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9A0A31-061D-4B92-BB8C-85D4C240E089}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9AD046-9055-420B-85AC-2179F5D6910C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="647" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="647" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Traffic Flows" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="270">
   <si>
     <t>Source Network</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Destination Protocol</t>
   </si>
   <si>
-    <t>Destination Port</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
     <t>UDP</t>
   </si>
   <si>
-    <t>ICMP</t>
-  </si>
-  <si>
     <t>any</t>
   </si>
   <si>
@@ -846,7 +840,22 @@
     <t>https, http, ssh</t>
   </si>
   <si>
-    <t>443, smtp</t>
+    <t>443, smtp, ldap</t>
+  </si>
+  <si>
+    <t>Destination Port or Application</t>
+  </si>
+  <si>
+    <t>icmp</t>
+  </si>
+  <si>
+    <t>icmp-ping</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>icmp-all</t>
   </si>
 </sst>
 </file>
@@ -1104,8 +1113,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1647,7 +1656,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1660,7 +1669,7 @@
     <col min="6" max="6" width="22.6640625" style="11" customWidth="1"/>
     <col min="7" max="7" width="28.6640625" style="8" customWidth="1"/>
     <col min="8" max="8" width="12.44140625" style="8" customWidth="1"/>
-    <col min="9" max="9" width="14" style="11" customWidth="1"/>
+    <col min="9" max="9" width="24.21875" style="11" customWidth="1"/>
     <col min="10" max="10" width="10.33203125" style="11" customWidth="1"/>
     <col min="11" max="11" width="9" style="8" customWidth="1"/>
     <col min="12" max="12" width="10.33203125" style="5" customWidth="1"/>
@@ -1669,306 +1678,306 @@
   <sheetData>
     <row r="1" spans="1:12" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>3</v>
+        <v>265</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="24" t="s">
-        <v>239</v>
+        <v>8</v>
+      </c>
+      <c r="I2" s="10">
+        <v>2345</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>9</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I8" s="10">
         <v>22</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2070,478 +2079,478 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B23" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B24" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B25" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B26" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B29" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B30" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B31" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B32" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B34" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B35" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B36" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B37" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B38" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B39" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B40" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B41" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B42" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B43" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B44" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B45" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B46" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B47" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B48" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B49" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B50" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B51" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B52" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B53" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B55" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B56" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B57" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B58" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2568,134 +2577,134 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C11" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2713,490 +2722,490 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.5546875" customWidth="1"/>
     <col min="2" max="2" width="9.5546875" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>239</v>
+        <v>269</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C2">
-        <v>179</v>
+        <v>266</v>
+      </c>
+      <c r="C2" s="24">
+        <v>999</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>230</v>
+        <v>267</v>
       </c>
       <c r="B3" t="s">
-        <v>190</v>
-      </c>
-      <c r="C3">
-        <v>68</v>
+        <v>266</v>
+      </c>
+      <c r="C3" s="24">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="B4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C4">
-        <v>67</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
       <c r="B5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C5">
-        <v>2401</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C6">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>229</v>
+        <v>245</v>
       </c>
       <c r="B7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C7">
-        <v>67</v>
+        <v>2401</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>252</v>
+        <v>226</v>
       </c>
       <c r="B8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C8">
-        <v>53</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="B9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C9">
-        <v>53</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>232</v>
+        <v>250</v>
       </c>
       <c r="B10" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C10">
-        <v>79</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>233</v>
+        <v>249</v>
       </c>
       <c r="B11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C11">
-        <v>80</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C12">
-        <v>443</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>250</v>
+        <v>231</v>
       </c>
       <c r="B13" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C13">
-        <v>500</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>253</v>
+        <v>232</v>
       </c>
       <c r="B14" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C14">
-        <v>4500</v>
+        <v>443</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>237</v>
+        <v>248</v>
       </c>
       <c r="B15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C15">
-        <v>143</v>
+        <v>500</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>238</v>
+        <v>251</v>
       </c>
       <c r="B16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C16">
-        <v>993</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C17">
-        <v>389</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="B18" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C18">
-        <v>646</v>
+        <v>993</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="B19" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C19">
-        <v>646</v>
+        <v>389</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B20" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C20">
-        <v>25</v>
+        <v>646</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="B21" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C21">
-        <v>1433</v>
+        <v>646</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B22" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C22">
-        <v>138</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B23" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C23">
-        <v>137</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>221</v>
+        <v>255</v>
       </c>
       <c r="B24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C24">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B25" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C25">
-        <v>111</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
       <c r="B26" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C26">
-        <v>2049</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="B27" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C27">
-        <v>2049</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="B28" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C28">
-        <v>123</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="B29" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C29">
-        <v>110</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="B30" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C30">
-        <v>1813</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B31" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C31">
-        <v>1812</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>261</v>
+        <v>242</v>
       </c>
       <c r="B32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C32">
-        <v>3389</v>
+        <v>1813</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>222</v>
+        <v>241</v>
       </c>
       <c r="B33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C33">
-        <v>445</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>225</v>
+        <v>259</v>
       </c>
       <c r="B34" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C34">
-        <v>25</v>
+        <v>3389</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>262</v>
+        <v>220</v>
       </c>
       <c r="B35" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C35">
-        <v>587</v>
+        <v>445</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>263</v>
+        <v>223</v>
       </c>
       <c r="B36" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C36">
-        <v>465</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>241</v>
+        <v>260</v>
       </c>
       <c r="B37" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C37">
-        <v>444</v>
+        <v>587</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B38" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C38">
-        <v>1434</v>
+        <v>465</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>260</v>
+        <v>239</v>
       </c>
       <c r="B39" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C39">
-        <v>1525</v>
+        <v>444</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>223</v>
+        <v>257</v>
       </c>
       <c r="B40" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C40">
-        <v>22</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>242</v>
+        <v>258</v>
       </c>
       <c r="B41" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C41">
-        <v>514</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B42" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C42">
-        <v>49</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="B43" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C43">
-        <v>65</v>
+        <v>514</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -3204,26 +3213,48 @@
         <v>224</v>
       </c>
       <c r="B44" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C44">
-        <v>23</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="B45" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C45">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>222</v>
+      </c>
+      <c r="B46" t="s">
+        <v>187</v>
+      </c>
+      <c r="C46">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>218</v>
+      </c>
+      <c r="B47" t="s">
+        <v>188</v>
+      </c>
+      <c r="C47">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C61">
-    <sortCondition ref="A2:A61"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C63">
+    <sortCondition ref="A4:A63"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3237,7 +3268,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3256,61 +3287,61 @@
         <v>2</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="17"/>
       <c r="B2" s="18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G2" s="17"/>
       <c r="H2" s="18" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17"/>
       <c r="B3" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G3" s="17"/>
       <c r="H3" s="18" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="19"/>
       <c r="B4" s="20" t="s">
-        <v>11</v>
+        <v>268</v>
       </c>
       <c r="G4" s="19"/>
       <c r="H4" s="20" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="2egXIuU8MC/uBPq9LD/l2KGbvWr/R96EIj4NJCfJ3AVlGxfchsvQ7CD+tvCD1GnWrIOC1ZrzGdJWUGI99vkjhg==" saltValue="4080Anc2sLS20VUJe4D8GQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3337,12 +3368,12 @@
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3350,7 +3381,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -3358,7 +3389,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -3366,7 +3397,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -3374,12 +3405,12 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -3387,7 +3418,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -3395,7 +3426,7 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -3403,7 +3434,7 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -3411,17 +3442,17 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -3429,7 +3460,7 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -3437,7 +3468,7 @@
         <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -3464,98 +3495,98 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Black and Lint all files
</commit_message>
<xml_diff>
--- a/fw_rules_test_02.xlsx
+++ b/fw_rules_test_02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\fw-rule-manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9AD046-9055-420B-85AC-2179F5D6910C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB12754-E47D-4724-8EED-890971A4D43C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="647" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1656,7 +1656,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1668,7 +1668,7 @@
     <col min="5" max="5" width="44.6640625" style="8" customWidth="1"/>
     <col min="6" max="6" width="22.6640625" style="11" customWidth="1"/>
     <col min="7" max="7" width="28.6640625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" style="8" customWidth="1"/>
     <col min="9" max="9" width="24.21875" style="11" customWidth="1"/>
     <col min="10" max="10" width="10.33203125" style="11" customWidth="1"/>
     <col min="11" max="11" width="9" style="8" customWidth="1"/>

</xml_diff>

<commit_message>
Added non-TCP or UDP protocols
</commit_message>
<xml_diff>
--- a/fw_rules_test_02.xlsx
+++ b/fw_rules_test_02.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\fw-rule-manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB12754-E47D-4724-8EED-890971A4D43C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6AFE77-2B99-4ECA-A1BF-55AF3501B8BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="647" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="647" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Traffic Flows" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Feedback" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Traffic Flows'!$A$1:$L$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Traffic Flows'!$A$1:$L$9</definedName>
     <definedName name="BulkData">'Dropdown Fields'!#REF!</definedName>
     <definedName name="Customer">'Dropdown Fields'!#REF!</definedName>
     <definedName name="DestinationProtocol">'Dropdown Fields'!#REF!</definedName>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="273">
   <si>
     <t>Source Network</t>
   </si>
@@ -204,9 +204,6 @@
     <t>In the "Traffic Flows" Worksheet, select the first usable cell in the column then CTRL+SHIFT+Down Arrow to select to last possible value in column</t>
   </si>
   <si>
-    <t>Management SSH</t>
-  </si>
-  <si>
     <t>SSH from Management Network</t>
   </si>
   <si>
@@ -555,12 +552,6 @@
     <t>InterAct application Client to Server</t>
   </si>
   <si>
-    <t>SSH access from Management Infra Services</t>
-  </si>
-  <si>
-    <t>Management SSH Infra Services</t>
-  </si>
-  <si>
     <t>Object Name</t>
   </si>
   <si>
@@ -684,12 +675,6 @@
     <t>#TODO</t>
   </si>
   <si>
-    <t>21, 44</t>
-  </si>
-  <si>
-    <t>443, 555-666</t>
-  </si>
-  <si>
     <t>review process ?</t>
   </si>
   <si>
@@ -837,9 +822,6 @@
     <t>Application</t>
   </si>
   <si>
-    <t>https, http, ssh</t>
-  </si>
-  <si>
     <t>443, smtp, ldap</t>
   </si>
   <si>
@@ -856,6 +838,33 @@
   </si>
   <si>
     <t>icmp-all</t>
+  </si>
+  <si>
+    <t>gre</t>
+  </si>
+  <si>
+    <t>icmpv6</t>
+  </si>
+  <si>
+    <t>ospf</t>
+  </si>
+  <si>
+    <t>Permit ICMP between customer zones</t>
+  </si>
+  <si>
+    <t>ssh, telnet, 830</t>
+  </si>
+  <si>
+    <t>Management access</t>
+  </si>
+  <si>
+    <t>Management SSH from Infra Services</t>
+  </si>
+  <si>
+    <t>https, 555-558</t>
+  </si>
+  <si>
+    <t>https, http</t>
   </si>
 </sst>
 </file>
@@ -1120,7 +1129,78 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="18">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1652,16 +1732,16 @@
     <tabColor rgb="FF33CC33"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30" style="8" customWidth="1"/>
+    <col min="1" max="1" width="32.88671875" style="8" customWidth="1"/>
     <col min="2" max="2" width="41.77734375" style="5" customWidth="1"/>
     <col min="3" max="3" width="10.21875" style="11" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" style="8" customWidth="1"/>
@@ -1702,13 +1782,13 @@
         <v>22</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>43</v>
@@ -1719,16 +1799,16 @@
         <v>24</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>47</v>
@@ -1737,13 +1817,13 @@
         <v>46</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I2" s="10">
-        <v>2345</v>
+        <v>8585</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>4</v>
@@ -1754,34 +1834,34 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>26</v>
+        <v>267</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>27</v>
+        <v>167</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>36</v>
+        <v>200</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>48</v>
+        <v>200</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>9</v>
+        <v>262</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>4</v>
@@ -1792,34 +1872,34 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>203</v>
+        <v>36</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>175</v>
+        <v>10</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>203</v>
+        <v>48</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>213</v>
+        <v>271</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>4</v>
@@ -1839,25 +1919,25 @@
         <v>10</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>31</v>
+        <v>200</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>172</v>
+        <v>53</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>8</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>4</v>
@@ -1868,34 +1948,34 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>177</v>
+        <v>23</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>178</v>
+        <v>23</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>47</v>
+        <v>201</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>215</v>
+        <v>172</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>10</v>
+        <v>169</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>8</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>212</v>
+        <v>258</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>4</v>
@@ -1906,10 +1986,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>52</v>
+        <v>174</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>10</v>
@@ -1918,10 +1998,10 @@
         <v>47</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>10</v>
+        <v>210</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>173</v>
+        <v>36</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>10</v>
@@ -1929,11 +2009,11 @@
       <c r="H7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="10" t="s">
-        <v>221</v>
+      <c r="I7" s="10">
+        <v>21</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>4</v>
@@ -1944,10 +2024,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>170</v>
+        <v>269</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>169</v>
+        <v>52</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>10</v>
@@ -1956,10 +2036,10 @@
         <v>47</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>167</v>
+        <v>10</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>47</v>
+        <v>170</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>10</v>
@@ -1967,11 +2047,11 @@
       <c r="H8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="10">
-        <v>22</v>
+      <c r="I8" s="10" t="s">
+        <v>268</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>4</v>
@@ -1980,59 +2060,134 @@
         <v>7</v>
       </c>
     </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="10">
+        <v>22</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L8" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="K2:K1048576">
-    <cfRule type="cellIs" dxfId="8" priority="4296" operator="equal">
+  <autoFilter ref="A1:L9" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="K10:K1048576">
+    <cfRule type="cellIs" dxfId="17" priority="4305" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="4297" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="4306" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L8">
-    <cfRule type="cellIs" dxfId="6" priority="31" operator="equal">
+  <conditionalFormatting sqref="L3:L9">
+    <cfRule type="cellIs" dxfId="15" priority="40" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="41" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D8">
-    <cfRule type="cellIs" dxfId="4" priority="10" operator="equal">
+  <conditionalFormatting sqref="D3:D9">
+    <cfRule type="cellIs" dxfId="13" priority="19" operator="equal">
       <formula>"any"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F8">
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
+  <conditionalFormatting sqref="F3:F9">
+    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
       <formula>"any"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J8">
+  <conditionalFormatting sqref="J3:J9">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+      <formula>"deny"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>"reject"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="4308" operator="equal">
+      <formula>"permit"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K9">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>"any"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"any"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"deny"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"reject"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4299" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
       <formula>"permit"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K9:K1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K10:K1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>INDIRECT("Boolean[Column1]")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:D1048576 C2:C8 H9:H1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:D1048576 H10:H1048576 C2:C9" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>INDIRECT("DestProtoTable[Column1]")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9:A1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A10:A1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>INDIRECT("ServiceTable[Column1]")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H8" xr:uid="{4D4FF7E8-FB77-4CF0-8941-3A2929C41218}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H9" xr:uid="{4D4FF7E8-FB77-4CF0-8941-3A2929C41218}">
       <formula1>INDIRECT("DestProtoTable[Values]")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:L8" xr:uid="{2459F31B-84F4-40B3-8182-C99B6AF8BAD6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:L9" xr:uid="{2459F31B-84F4-40B3-8182-C99B6AF8BAD6}">
       <formula1>INDIRECT("Boolean[Values]")</formula1>
     </dataValidation>
   </dataValidations>
@@ -2045,13 +2200,13 @@
           <x14:formula1>
             <xm:f>Zones!$A$2:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F8 D2:D8</xm:sqref>
+          <xm:sqref>D2:D9 F2:F9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FD155D18-2081-4233-B9F7-E634676BB1FE}">
           <x14:formula1>
             <xm:f>'Dropdown Fields'!$H$2:$H$4</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J8</xm:sqref>
+          <xm:sqref>J2:J9</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2079,10 +2234,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>3</v>
@@ -2090,467 +2245,467 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
         <v>56</v>
-      </c>
-      <c r="B3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
         <v>58</v>
       </c>
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
       <c r="C4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
         <v>60</v>
       </c>
-      <c r="B5" t="s">
-        <v>61</v>
-      </c>
       <c r="C5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
         <v>62</v>
-      </c>
-      <c r="B6" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" t="s">
         <v>65</v>
-      </c>
-      <c r="B8" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" t="s">
         <v>67</v>
-      </c>
-      <c r="B9" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" t="s">
         <v>71</v>
-      </c>
-      <c r="B12" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" t="s">
         <v>73</v>
-      </c>
-      <c r="B13" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" t="s">
         <v>75</v>
-      </c>
-      <c r="B14" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" t="s">
         <v>77</v>
-      </c>
-      <c r="B15" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" t="s">
         <v>79</v>
-      </c>
-      <c r="B16" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" t="s">
         <v>81</v>
-      </c>
-      <c r="B17" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" t="s">
         <v>83</v>
-      </c>
-      <c r="B18" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" t="s">
         <v>85</v>
-      </c>
-      <c r="B19" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" t="s">
         <v>87</v>
-      </c>
-      <c r="B20" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" t="s">
         <v>89</v>
-      </c>
-      <c r="B21" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" t="s">
         <v>91</v>
-      </c>
-      <c r="B22" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B23" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" t="s">
         <v>94</v>
-      </c>
-      <c r="B24" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" t="s">
         <v>96</v>
-      </c>
-      <c r="B25" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" t="s">
         <v>98</v>
-      </c>
-      <c r="B26" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" t="s">
         <v>100</v>
-      </c>
-      <c r="B27" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" t="s">
         <v>102</v>
-      </c>
-      <c r="B28" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" t="s">
         <v>104</v>
-      </c>
-      <c r="B29" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" t="s">
         <v>106</v>
-      </c>
-      <c r="B30" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>107</v>
+      </c>
+      <c r="B31" t="s">
         <v>108</v>
-      </c>
-      <c r="B31" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>109</v>
+      </c>
+      <c r="B32" t="s">
         <v>110</v>
-      </c>
-      <c r="B32" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>111</v>
+      </c>
+      <c r="B33" t="s">
         <v>112</v>
-      </c>
-      <c r="B33" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>113</v>
+      </c>
+      <c r="B34" t="s">
         <v>114</v>
-      </c>
-      <c r="B34" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35" t="s">
         <v>116</v>
-      </c>
-      <c r="B35" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" t="s">
         <v>118</v>
-      </c>
-      <c r="B36" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>119</v>
+      </c>
+      <c r="B37" t="s">
         <v>120</v>
-      </c>
-      <c r="B37" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>121</v>
+      </c>
+      <c r="B38" t="s">
         <v>122</v>
-      </c>
-      <c r="B38" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>123</v>
+      </c>
+      <c r="B39" t="s">
         <v>124</v>
-      </c>
-      <c r="B39" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>125</v>
+      </c>
+      <c r="B40" t="s">
         <v>126</v>
-      </c>
-      <c r="B40" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>127</v>
+      </c>
+      <c r="B41" t="s">
         <v>128</v>
-      </c>
-      <c r="B41" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>129</v>
+      </c>
+      <c r="B42" t="s">
         <v>130</v>
-      </c>
-      <c r="B42" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" t="s">
         <v>132</v>
-      </c>
-      <c r="B43" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>133</v>
+      </c>
+      <c r="B44" t="s">
         <v>134</v>
-      </c>
-      <c r="B44" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>135</v>
+      </c>
+      <c r="B45" t="s">
         <v>136</v>
-      </c>
-      <c r="B45" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>137</v>
+      </c>
+      <c r="B46" t="s">
         <v>138</v>
-      </c>
-      <c r="B46" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>139</v>
+      </c>
+      <c r="B47" t="s">
         <v>140</v>
-      </c>
-      <c r="B47" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>141</v>
+      </c>
+      <c r="B48" t="s">
         <v>142</v>
-      </c>
-      <c r="B48" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>143</v>
+      </c>
+      <c r="B49" t="s">
         <v>144</v>
-      </c>
-      <c r="B49" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>145</v>
+      </c>
+      <c r="B50" t="s">
         <v>146</v>
-      </c>
-      <c r="B50" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>147</v>
+      </c>
+      <c r="B51" t="s">
         <v>148</v>
-      </c>
-      <c r="B51" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>149</v>
+      </c>
+      <c r="B52" t="s">
         <v>150</v>
-      </c>
-      <c r="B52" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B53" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>152</v>
+      </c>
+      <c r="B54" t="s">
         <v>153</v>
-      </c>
-      <c r="B54" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>154</v>
+      </c>
+      <c r="B55" t="s">
         <v>155</v>
-      </c>
-      <c r="B55" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>156</v>
+      </c>
+      <c r="B56" t="s">
         <v>157</v>
-      </c>
-      <c r="B56" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>158</v>
+      </c>
+      <c r="B57" t="s">
         <v>159</v>
-      </c>
-      <c r="B57" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
+        <v>160</v>
+      </c>
+      <c r="B58" t="s">
         <v>161</v>
-      </c>
-      <c r="B58" t="s">
-        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2577,10 +2732,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C1" t="s">
         <v>25</v>
@@ -2588,24 +2743,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C3" t="s">
         <v>198</v>
-      </c>
-      <c r="C3" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2687,13 +2842,13 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C11" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -2722,10 +2877,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2737,21 +2892,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>22</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="B2" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C2" s="24">
         <v>999</v>
@@ -2759,10 +2914,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B3" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C3" s="24">
         <v>0</v>
@@ -2770,54 +2925,54 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>237</v>
+        <v>265</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
-      </c>
-      <c r="C4">
-        <v>179</v>
+        <v>265</v>
+      </c>
+      <c r="C4" s="24">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>228</v>
+        <v>264</v>
       </c>
       <c r="B5" t="s">
-        <v>188</v>
-      </c>
-      <c r="C5">
-        <v>68</v>
+        <v>264</v>
+      </c>
+      <c r="C5" s="24">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>229</v>
+        <v>266</v>
       </c>
       <c r="B6" t="s">
-        <v>188</v>
-      </c>
-      <c r="C6">
-        <v>67</v>
+        <v>266</v>
+      </c>
+      <c r="C6" s="24">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="B7" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C7">
-        <v>2401</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B8" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C8">
         <v>68</v>
@@ -2825,10 +2980,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B9" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C9">
         <v>67</v>
@@ -2836,425 +2991,458 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="B10" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C10">
-        <v>53</v>
+        <v>2401</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>249</v>
+        <v>221</v>
       </c>
       <c r="B11" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C11">
-        <v>53</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C12">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>231</v>
+        <v>245</v>
       </c>
       <c r="B13" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C13">
-        <v>80</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="B14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C14">
-        <v>443</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>248</v>
+        <v>225</v>
       </c>
       <c r="B15" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C15">
-        <v>500</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>251</v>
+        <v>226</v>
       </c>
       <c r="B16" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C16">
-        <v>4500</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="B17" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C17">
-        <v>143</v>
+        <v>443</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="B18" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C18">
-        <v>993</v>
+        <v>500</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="B19" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C19">
-        <v>389</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="B20" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C20">
-        <v>646</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="B21" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C21">
-        <v>646</v>
+        <v>993</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>252</v>
+        <v>233</v>
       </c>
       <c r="B22" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C22">
-        <v>25</v>
+        <v>389</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="B23" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C23">
-        <v>1433</v>
+        <v>646</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="B24" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C24">
-        <v>138</v>
+        <v>646</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="B25" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C25">
-        <v>137</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>219</v>
+        <v>248</v>
       </c>
       <c r="B26" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C26">
-        <v>139</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C27">
-        <v>111</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="B28" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C28">
-        <v>2049</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>244</v>
+        <v>214</v>
       </c>
       <c r="B29" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C29">
-        <v>2049</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>234</v>
+        <v>251</v>
       </c>
       <c r="B30" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C30">
-        <v>123</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="B31" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C31">
-        <v>110</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B32" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C32">
-        <v>1813</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="B33" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C33">
-        <v>1812</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>259</v>
+        <v>228</v>
       </c>
       <c r="B34" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C34">
-        <v>3389</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>220</v>
+        <v>237</v>
       </c>
       <c r="B35" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C35">
-        <v>445</v>
+        <v>1813</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>223</v>
+        <v>236</v>
       </c>
       <c r="B36" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C36">
-        <v>25</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B37" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C37">
-        <v>587</v>
+        <v>3389</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>261</v>
+        <v>215</v>
       </c>
       <c r="B38" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C38">
-        <v>465</v>
+        <v>445</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>239</v>
+        <v>218</v>
       </c>
       <c r="B39" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C39">
-        <v>444</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B40" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C40">
-        <v>1434</v>
+        <v>587</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B41" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C41">
-        <v>1525</v>
+        <v>465</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c r="B42" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C42">
-        <v>22</v>
+        <v>444</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>240</v>
+        <v>252</v>
       </c>
       <c r="B43" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C43">
-        <v>514</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>224</v>
+        <v>253</v>
       </c>
       <c r="B44" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C44">
-        <v>49</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="B45" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C45">
-        <v>65</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="B46" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C46">
-        <v>23</v>
+        <v>514</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B47" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C47">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>220</v>
+      </c>
+      <c r="B48" t="s">
+        <v>184</v>
+      </c>
+      <c r="C48">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>217</v>
+      </c>
+      <c r="B49" t="s">
+        <v>184</v>
+      </c>
+      <c r="C49">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>213</v>
+      </c>
+      <c r="B50" t="s">
+        <v>185</v>
+      </c>
+      <c r="C50">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C63">
-    <sortCondition ref="A4:A63"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C66">
+    <sortCondition ref="A7:A66"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3287,19 +3475,19 @@
         <v>2</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -3313,7 +3501,7 @@
       </c>
       <c r="G2" s="17"/>
       <c r="H2" s="18" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3327,17 +3515,17 @@
       </c>
       <c r="G3" s="17"/>
       <c r="H3" s="18" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="19"/>
       <c r="B4" s="20" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="G4" s="19"/>
       <c r="H4" s="20" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -3495,98 +3683,98 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B10" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>